<commit_message>
450 DSA Kadanne Algo
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\Desktop\Git\Codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\Desktop\450 DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0EFB6E-790F-46DF-9398-03AB8BF9F870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E3BE94-3E87-4D33-B08B-0E778CBFDF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1856,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1976,7 +1976,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Added and Solved Largest Subarray with sum Zero in 450 DSA Solved using Hashing
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\Desktop\450 DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE49C92-B36D-4663-B937-B698BA7D35DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5D5887-7DD0-48B1-9069-6F376B2ECE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="471">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1435,6 +1435,9 @@
   </si>
   <si>
     <t>4 Sum from Striver</t>
+  </si>
+  <si>
+    <t>Largest Subarray with zero Sum from Striver</t>
   </si>
 </sst>
 </file>
@@ -1865,7 +1868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -2330,9 +2333,15 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">
-      <c r="A45" s="4"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="3"/>
+      <c r="A45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="21">
       <c r="A46" s="4"/>

</xml_diff>

<commit_message>
Solved three Question in 450 DSA 1) Reverse a String 2) Check whether a String is Palindrome or not 3) Find Duplicate character in a string
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\Desktop\450 DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E5C3B9-E04D-4E93-B185-0D23137F5DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B942E4A6-CC2E-45D9-BD08-117F0B38A8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1883,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C487"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2513,7 +2513,7 @@
         <v>53</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="21">
@@ -2524,7 +2524,7 @@
         <v>54</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="21">
@@ -2535,7 +2535,7 @@
         <v>55</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Added and Solved 2 Question from Striver in 450 DSA Sheet 1) Reverse a Linked List 2)Find Middle of the Linked List (Through Tortoise and Rabbit method)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\Desktop\450 DSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1316eb900441c6a3/Desktop/450 DSA and 30 Day Striver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B942E4A6-CC2E-45D9-BD08-117F0B38A8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{B942E4A6-CC2E-45D9-BD08-117F0B38A8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDCBD13C-2C70-4830-8851-F19ECDD29B30}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="474">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1444,6 +1444,9 @@
   </si>
   <si>
     <t>Count the number of subarrays having a given XOR from Striver</t>
+  </si>
+  <si>
+    <t>Find Middle of the Linked List</t>
   </si>
 </sst>
 </file>
@@ -1881,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:C487"/>
+  <dimension ref="A1:C488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3391,7 +3394,7 @@
         <v>134</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21">
@@ -3779,27 +3782,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="21">
-      <c r="B182" s="6"/>
-      <c r="C182" s="3"/>
+    <row r="181" spans="1:3" ht="19.5">
+      <c r="A181" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B181" t="s">
+        <v>473</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="183" spans="1:3" ht="21">
-      <c r="A183" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B183" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B183" s="6"/>
+      <c r="C183" s="3"/>
     </row>
     <row r="184" spans="1:3" ht="21">
       <c r="A184" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>3</v>
@@ -3810,7 +3813,7 @@
         <v>170</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>3</v>
@@ -3821,7 +3824,7 @@
         <v>170</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>3</v>
@@ -3832,7 +3835,7 @@
         <v>170</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>3</v>
@@ -3843,7 +3846,7 @@
         <v>170</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>3</v>
@@ -3854,7 +3857,7 @@
         <v>170</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>3</v>
@@ -3865,7 +3868,7 @@
         <v>170</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>3</v>
@@ -3876,7 +3879,7 @@
         <v>170</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>3</v>
@@ -3887,7 +3890,7 @@
         <v>170</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>3</v>
@@ -3898,7 +3901,7 @@
         <v>170</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>3</v>
@@ -3909,7 +3912,7 @@
         <v>170</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>3</v>
@@ -3920,7 +3923,7 @@
         <v>170</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>3</v>
@@ -3931,7 +3934,7 @@
         <v>170</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>3</v>
@@ -3942,7 +3945,7 @@
         <v>170</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>3</v>
@@ -3953,7 +3956,7 @@
         <v>170</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>3</v>
@@ -3964,7 +3967,7 @@
         <v>170</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>3</v>
@@ -3975,7 +3978,7 @@
         <v>170</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>3</v>
@@ -3986,7 +3989,7 @@
         <v>170</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>3</v>
@@ -3997,7 +4000,7 @@
         <v>170</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C202" s="3" t="s">
         <v>3</v>
@@ -4008,7 +4011,7 @@
         <v>170</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>3</v>
@@ -4019,7 +4022,7 @@
         <v>170</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>3</v>
@@ -4030,7 +4033,7 @@
         <v>170</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>3</v>
@@ -4041,7 +4044,7 @@
         <v>170</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>3</v>
@@ -4052,7 +4055,7 @@
         <v>170</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>3</v>
@@ -4063,7 +4066,7 @@
         <v>170</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>3</v>
@@ -4074,7 +4077,7 @@
         <v>170</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>3</v>
@@ -4085,7 +4088,7 @@
         <v>170</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>3</v>
@@ -4096,7 +4099,7 @@
         <v>170</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>3</v>
@@ -4107,7 +4110,7 @@
         <v>170</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>3</v>
@@ -4118,7 +4121,7 @@
         <v>170</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>3</v>
@@ -4129,7 +4132,7 @@
         <v>170</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>3</v>
@@ -4140,7 +4143,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>3</v>
@@ -4151,7 +4154,7 @@
         <v>170</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>3</v>
@@ -4162,16 +4165,22 @@
         <v>170</v>
       </c>
       <c r="B217" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="21">
+      <c r="A218" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B218" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C217" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="21">
-      <c r="A218" s="7"/>
-      <c r="B218" s="6"/>
-      <c r="C218" s="3"/>
+      <c r="C218" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="219" spans="1:3" ht="21">
       <c r="A219" s="7"/>
@@ -4179,22 +4188,16 @@
       <c r="C219" s="3"/>
     </row>
     <row r="220" spans="1:3" ht="21">
-      <c r="A220" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B220" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A220" s="7"/>
+      <c r="B220" s="6"/>
+      <c r="C220" s="3"/>
     </row>
     <row r="221" spans="1:3" ht="21">
       <c r="A221" s="4" t="s">
         <v>206</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>3</v>
@@ -4205,7 +4208,7 @@
         <v>206</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>3</v>
@@ -4216,7 +4219,7 @@
         <v>206</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>3</v>
@@ -4227,7 +4230,7 @@
         <v>206</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>3</v>
@@ -4238,7 +4241,7 @@
         <v>206</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>3</v>
@@ -4248,8 +4251,8 @@
       <c r="A226" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B226" s="8" t="s">
-        <v>213</v>
+      <c r="B226" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>3</v>
@@ -4259,8 +4262,8 @@
       <c r="A227" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B227" s="5" t="s">
-        <v>214</v>
+      <c r="B227" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>3</v>
@@ -4271,7 +4274,7 @@
         <v>206</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C228" s="3" t="s">
         <v>3</v>
@@ -4282,7 +4285,7 @@
         <v>206</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>3</v>
@@ -4293,7 +4296,7 @@
         <v>206</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>3</v>
@@ -4304,7 +4307,7 @@
         <v>206</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>3</v>
@@ -4315,7 +4318,7 @@
         <v>206</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>3</v>
@@ -4326,7 +4329,7 @@
         <v>206</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>3</v>
@@ -4337,7 +4340,7 @@
         <v>206</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>3</v>
@@ -4348,7 +4351,7 @@
         <v>206</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>3</v>
@@ -4359,7 +4362,7 @@
         <v>206</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>3</v>
@@ -4370,7 +4373,7 @@
         <v>206</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>3</v>
@@ -4381,7 +4384,7 @@
         <v>206</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>3</v>
@@ -4392,7 +4395,7 @@
         <v>206</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>3</v>
@@ -4403,7 +4406,7 @@
         <v>206</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>3</v>
@@ -4414,37 +4417,37 @@
         <v>206</v>
       </c>
       <c r="B241" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" ht="21">
+      <c r="A242" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B242" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C241" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" ht="21">
-      <c r="B242" s="6"/>
-      <c r="C242" s="3"/>
+      <c r="C242" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="243" spans="1:3" ht="21">
       <c r="B243" s="6"/>
       <c r="C243" s="3"/>
     </row>
     <row r="244" spans="1:3" ht="21">
-      <c r="A244" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B244" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="C244" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B244" s="6"/>
+      <c r="C244" s="3"/>
     </row>
     <row r="245" spans="1:3" ht="21">
       <c r="A245" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>3</v>
@@ -4455,7 +4458,7 @@
         <v>229</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>3</v>
@@ -4466,7 +4469,7 @@
         <v>229</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>3</v>
@@ -4477,7 +4480,7 @@
         <v>229</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>3</v>
@@ -4488,7 +4491,7 @@
         <v>229</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>3</v>
@@ -4499,7 +4502,7 @@
         <v>229</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C250" s="3" t="s">
         <v>3</v>
@@ -4510,7 +4513,7 @@
         <v>229</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C251" s="3" t="s">
         <v>3</v>
@@ -4521,7 +4524,7 @@
         <v>229</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C252" s="3" t="s">
         <v>3</v>
@@ -4532,7 +4535,7 @@
         <v>229</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C253" s="3" t="s">
         <v>3</v>
@@ -4543,7 +4546,7 @@
         <v>229</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>3</v>
@@ -4554,7 +4557,7 @@
         <v>229</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>3</v>
@@ -4565,7 +4568,7 @@
         <v>229</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>3</v>
@@ -4576,7 +4579,7 @@
         <v>229</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>3</v>
@@ -4587,7 +4590,7 @@
         <v>229</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>3</v>
@@ -4598,7 +4601,7 @@
         <v>229</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>3</v>
@@ -4609,7 +4612,7 @@
         <v>229</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>3</v>
@@ -4620,7 +4623,7 @@
         <v>229</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>3</v>
@@ -4631,7 +4634,7 @@
         <v>229</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C262" s="3" t="s">
         <v>3</v>
@@ -4642,7 +4645,7 @@
         <v>229</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>3</v>
@@ -4653,7 +4656,7 @@
         <v>229</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C264" s="3" t="s">
         <v>3</v>
@@ -4664,7 +4667,7 @@
         <v>229</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>3</v>
@@ -4675,7 +4678,7 @@
         <v>229</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>3</v>
@@ -4686,7 +4689,7 @@
         <v>229</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>3</v>
@@ -4697,7 +4700,7 @@
         <v>229</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C268" s="3" t="s">
         <v>3</v>
@@ -4708,7 +4711,7 @@
         <v>229</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C269" s="3" t="s">
         <v>3</v>
@@ -4719,7 +4722,7 @@
         <v>229</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C270" s="3" t="s">
         <v>3</v>
@@ -4730,7 +4733,7 @@
         <v>229</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C271" s="3" t="s">
         <v>3</v>
@@ -4741,7 +4744,7 @@
         <v>229</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>3</v>
@@ -4752,7 +4755,7 @@
         <v>229</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>3</v>
@@ -4763,7 +4766,7 @@
         <v>229</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C274" s="3" t="s">
         <v>3</v>
@@ -4774,7 +4777,7 @@
         <v>229</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>3</v>
@@ -4785,7 +4788,7 @@
         <v>229</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C276" s="3" t="s">
         <v>3</v>
@@ -4796,7 +4799,7 @@
         <v>229</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>86</v>
+        <v>262</v>
       </c>
       <c r="C277" s="3" t="s">
         <v>3</v>
@@ -4807,37 +4810,37 @@
         <v>229</v>
       </c>
       <c r="B278" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C278" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" ht="21">
+      <c r="A279" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B279" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C278" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" ht="21">
-      <c r="B279" s="6"/>
-      <c r="C279" s="3"/>
+      <c r="C279" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="280" spans="1:3" ht="21">
       <c r="B280" s="6"/>
       <c r="C280" s="3"/>
     </row>
     <row r="281" spans="1:3" ht="21">
-      <c r="A281" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B281" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C281" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B281" s="6"/>
+      <c r="C281" s="3"/>
     </row>
     <row r="282" spans="1:3" ht="21">
       <c r="A282" s="4" t="s">
         <v>264</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>3</v>
@@ -4848,7 +4851,7 @@
         <v>264</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>3</v>
@@ -4859,7 +4862,7 @@
         <v>264</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>3</v>
@@ -4870,7 +4873,7 @@
         <v>264</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C285" s="3" t="s">
         <v>3</v>
@@ -4881,7 +4884,7 @@
         <v>264</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C286" s="3" t="s">
         <v>3</v>
@@ -4892,7 +4895,7 @@
         <v>264</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C287" s="3" t="s">
         <v>3</v>
@@ -4903,7 +4906,7 @@
         <v>264</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>3</v>
@@ -4914,7 +4917,7 @@
         <v>264</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C289" s="3" t="s">
         <v>3</v>
@@ -4925,7 +4928,7 @@
         <v>264</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C290" s="3" t="s">
         <v>3</v>
@@ -4936,7 +4939,7 @@
         <v>264</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>3</v>
@@ -4947,7 +4950,7 @@
         <v>264</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>3</v>
@@ -4958,7 +4961,7 @@
         <v>264</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C293" s="3" t="s">
         <v>3</v>
@@ -4969,7 +4972,7 @@
         <v>264</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C294" s="3" t="s">
         <v>3</v>
@@ -4980,7 +4983,7 @@
         <v>264</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C295" s="3" t="s">
         <v>3</v>
@@ -4991,7 +4994,7 @@
         <v>264</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C296" s="3" t="s">
         <v>3</v>
@@ -5002,7 +5005,7 @@
         <v>264</v>
       </c>
       <c r="B297" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C297" s="3" t="s">
         <v>3</v>
@@ -5013,7 +5016,7 @@
         <v>264</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C298" s="3" t="s">
         <v>3</v>
@@ -5024,37 +5027,37 @@
         <v>264</v>
       </c>
       <c r="B299" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C299" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" ht="21">
+      <c r="A300" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B300" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C299" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" ht="21">
-      <c r="B300" s="6"/>
-      <c r="C300" s="3"/>
+      <c r="C300" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="301" spans="1:3" ht="21">
       <c r="B301" s="6"/>
       <c r="C301" s="3"/>
     </row>
     <row r="302" spans="1:3" ht="21">
-      <c r="A302" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B302" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="C302" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B302" s="6"/>
+      <c r="C302" s="3"/>
     </row>
     <row r="303" spans="1:3" ht="21">
       <c r="A303" s="4" t="s">
         <v>284</v>
       </c>
       <c r="B303" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C303" s="3" t="s">
         <v>3</v>
@@ -5065,7 +5068,7 @@
         <v>284</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C304" s="3" t="s">
         <v>3</v>
@@ -5076,7 +5079,7 @@
         <v>284</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C305" s="3" t="s">
         <v>3</v>
@@ -5087,7 +5090,7 @@
         <v>284</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C306" s="3" t="s">
         <v>3</v>
@@ -5098,7 +5101,7 @@
         <v>284</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C307" s="3" t="s">
         <v>3</v>
@@ -5109,7 +5112,7 @@
         <v>284</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C308" s="3" t="s">
         <v>3</v>
@@ -5120,7 +5123,7 @@
         <v>284</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C309" s="3" t="s">
         <v>3</v>
@@ -5131,7 +5134,7 @@
         <v>284</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C310" s="3" t="s">
         <v>3</v>
@@ -5142,7 +5145,7 @@
         <v>284</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C311" s="3" t="s">
         <v>3</v>
@@ -5153,7 +5156,7 @@
         <v>284</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>3</v>
@@ -5164,7 +5167,7 @@
         <v>284</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C313" s="3" t="s">
         <v>3</v>
@@ -5175,7 +5178,7 @@
         <v>284</v>
       </c>
       <c r="B314" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>3</v>
@@ -5185,8 +5188,8 @@
       <c r="A315" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B315" s="8" t="s">
-        <v>298</v>
+      <c r="B315" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>3</v>
@@ -5196,8 +5199,8 @@
       <c r="A316" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B316" s="5" t="s">
-        <v>299</v>
+      <c r="B316" s="8" t="s">
+        <v>298</v>
       </c>
       <c r="C316" s="3" t="s">
         <v>3</v>
@@ -5208,7 +5211,7 @@
         <v>284</v>
       </c>
       <c r="B317" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>3</v>
@@ -5219,7 +5222,7 @@
         <v>284</v>
       </c>
       <c r="B318" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>3</v>
@@ -5230,7 +5233,7 @@
         <v>284</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>3</v>
@@ -5241,7 +5244,7 @@
         <v>284</v>
       </c>
       <c r="B320" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C320" s="3" t="s">
         <v>3</v>
@@ -5252,7 +5255,7 @@
         <v>284</v>
       </c>
       <c r="B321" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C321" s="3" t="s">
         <v>3</v>
@@ -5263,7 +5266,7 @@
         <v>284</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C322" s="3" t="s">
         <v>3</v>
@@ -5274,7 +5277,7 @@
         <v>284</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C323" s="3" t="s">
         <v>3</v>
@@ -5285,7 +5288,7 @@
         <v>284</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C324" s="3" t="s">
         <v>3</v>
@@ -5296,7 +5299,7 @@
         <v>284</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C325" s="3" t="s">
         <v>3</v>
@@ -5307,7 +5310,7 @@
         <v>284</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>3</v>
@@ -5318,7 +5321,7 @@
         <v>284</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C327" s="3" t="s">
         <v>3</v>
@@ -5329,7 +5332,7 @@
         <v>284</v>
       </c>
       <c r="B328" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>3</v>
@@ -5340,7 +5343,7 @@
         <v>284</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C329" s="3" t="s">
         <v>3</v>
@@ -5351,7 +5354,7 @@
         <v>284</v>
       </c>
       <c r="B330" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C330" s="3" t="s">
         <v>3</v>
@@ -5362,7 +5365,7 @@
         <v>284</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C331" s="3" t="s">
         <v>3</v>
@@ -5373,7 +5376,7 @@
         <v>284</v>
       </c>
       <c r="B332" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>3</v>
@@ -5384,7 +5387,7 @@
         <v>284</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C333" s="3" t="s">
         <v>3</v>
@@ -5395,7 +5398,7 @@
         <v>284</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C334" s="3" t="s">
         <v>3</v>
@@ -5406,7 +5409,7 @@
         <v>284</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C335" s="3" t="s">
         <v>3</v>
@@ -5417,7 +5420,7 @@
         <v>284</v>
       </c>
       <c r="B336" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C336" s="3" t="s">
         <v>3</v>
@@ -5428,7 +5431,7 @@
         <v>284</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C337" s="3" t="s">
         <v>3</v>
@@ -5439,7 +5442,7 @@
         <v>284</v>
       </c>
       <c r="B338" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C338" s="3" t="s">
         <v>3</v>
@@ -5450,37 +5453,37 @@
         <v>284</v>
       </c>
       <c r="B339" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" ht="21">
+      <c r="A340" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B340" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="C339" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="340" spans="1:3" ht="21">
-      <c r="B340" s="6"/>
-      <c r="C340" s="3"/>
+      <c r="C340" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="341" spans="1:3" ht="21">
       <c r="B341" s="6"/>
       <c r="C341" s="3"/>
     </row>
     <row r="342" spans="1:3" ht="21">
-      <c r="A342" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B342" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="C342" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B342" s="6"/>
+      <c r="C342" s="3"/>
     </row>
     <row r="343" spans="1:3" ht="21">
       <c r="A343" s="7" t="s">
         <v>323</v>
       </c>
       <c r="B343" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C343" s="3" t="s">
         <v>3</v>
@@ -5491,7 +5494,7 @@
         <v>323</v>
       </c>
       <c r="B344" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>3</v>
@@ -5502,7 +5505,7 @@
         <v>323</v>
       </c>
       <c r="B345" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C345" s="3" t="s">
         <v>3</v>
@@ -5513,7 +5516,7 @@
         <v>323</v>
       </c>
       <c r="B346" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C346" s="3" t="s">
         <v>3</v>
@@ -5524,7 +5527,7 @@
         <v>323</v>
       </c>
       <c r="B347" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C347" s="3" t="s">
         <v>3</v>
@@ -5535,7 +5538,7 @@
         <v>323</v>
       </c>
       <c r="B348" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C348" s="3" t="s">
         <v>3</v>
@@ -5546,7 +5549,7 @@
         <v>323</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>3</v>
@@ -5556,8 +5559,8 @@
       <c r="A350" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B350" s="8" t="s">
-        <v>332</v>
+      <c r="B350" s="5" t="s">
+        <v>331</v>
       </c>
       <c r="C350" s="3" t="s">
         <v>3</v>
@@ -5567,8 +5570,8 @@
       <c r="A351" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B351" s="5" t="s">
-        <v>333</v>
+      <c r="B351" s="8" t="s">
+        <v>332</v>
       </c>
       <c r="C351" s="3" t="s">
         <v>3</v>
@@ -5579,7 +5582,7 @@
         <v>323</v>
       </c>
       <c r="B352" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C352" s="3" t="s">
         <v>3</v>
@@ -5590,7 +5593,7 @@
         <v>323</v>
       </c>
       <c r="B353" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C353" s="3" t="s">
         <v>3</v>
@@ -5601,7 +5604,7 @@
         <v>323</v>
       </c>
       <c r="B354" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C354" s="3" t="s">
         <v>3</v>
@@ -5612,7 +5615,7 @@
         <v>323</v>
       </c>
       <c r="B355" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C355" s="3" t="s">
         <v>3</v>
@@ -5623,7 +5626,7 @@
         <v>323</v>
       </c>
       <c r="B356" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>3</v>
@@ -5634,7 +5637,7 @@
         <v>323</v>
       </c>
       <c r="B357" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C357" s="3" t="s">
         <v>3</v>
@@ -5645,7 +5648,7 @@
         <v>323</v>
       </c>
       <c r="B358" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C358" s="3" t="s">
         <v>3</v>
@@ -5656,37 +5659,37 @@
         <v>323</v>
       </c>
       <c r="B359" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C359" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" ht="21">
+      <c r="A360" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B360" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="C359" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="360" spans="1:3" ht="21">
-      <c r="B360" s="6"/>
-      <c r="C360" s="3"/>
+      <c r="C360" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="B361" s="6"/>
       <c r="C361" s="3"/>
     </row>
     <row r="362" spans="1:3" ht="21">
-      <c r="A362" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B362" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="C362" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B362" s="6"/>
+      <c r="C362" s="3"/>
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="7" t="s">
         <v>342</v>
       </c>
       <c r="B363" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C363" s="3" t="s">
         <v>3</v>
@@ -5697,7 +5700,7 @@
         <v>342</v>
       </c>
       <c r="B364" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C364" s="3" t="s">
         <v>3</v>
@@ -5708,7 +5711,7 @@
         <v>342</v>
       </c>
       <c r="B365" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C365" s="3" t="s">
         <v>3</v>
@@ -5719,7 +5722,7 @@
         <v>342</v>
       </c>
       <c r="B366" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C366" s="3" t="s">
         <v>3</v>
@@ -5730,7 +5733,7 @@
         <v>342</v>
       </c>
       <c r="B367" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C367" s="3" t="s">
         <v>3</v>
@@ -5741,7 +5744,7 @@
         <v>342</v>
       </c>
       <c r="B368" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C368" s="3" t="s">
         <v>3</v>
@@ -5752,7 +5755,7 @@
         <v>342</v>
       </c>
       <c r="B369" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C369" s="3" t="s">
         <v>3</v>
@@ -5763,7 +5766,7 @@
         <v>342</v>
       </c>
       <c r="B370" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C370" s="3" t="s">
         <v>3</v>
@@ -5774,7 +5777,7 @@
         <v>342</v>
       </c>
       <c r="B371" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C371" s="3" t="s">
         <v>3</v>
@@ -5785,7 +5788,7 @@
         <v>342</v>
       </c>
       <c r="B372" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C372" s="3" t="s">
         <v>3</v>
@@ -5796,7 +5799,7 @@
         <v>342</v>
       </c>
       <c r="B373" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>3</v>
@@ -5807,7 +5810,7 @@
         <v>342</v>
       </c>
       <c r="B374" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>3</v>
@@ -5818,7 +5821,7 @@
         <v>342</v>
       </c>
       <c r="B375" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>3</v>
@@ -5829,7 +5832,7 @@
         <v>342</v>
       </c>
       <c r="B376" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>3</v>
@@ -5840,7 +5843,7 @@
         <v>342</v>
       </c>
       <c r="B377" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>3</v>
@@ -5851,7 +5854,7 @@
         <v>342</v>
       </c>
       <c r="B378" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C378" s="3" t="s">
         <v>3</v>
@@ -5862,7 +5865,7 @@
         <v>342</v>
       </c>
       <c r="B379" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C379" s="3" t="s">
         <v>3</v>
@@ -5873,7 +5876,7 @@
         <v>342</v>
       </c>
       <c r="B380" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C380" s="3" t="s">
         <v>3</v>
@@ -5884,7 +5887,7 @@
         <v>342</v>
       </c>
       <c r="B381" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C381" s="3" t="s">
         <v>3</v>
@@ -5895,7 +5898,7 @@
         <v>342</v>
       </c>
       <c r="B382" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C382" s="3" t="s">
         <v>3</v>
@@ -5906,7 +5909,7 @@
         <v>342</v>
       </c>
       <c r="B383" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C383" s="3" t="s">
         <v>3</v>
@@ -5917,7 +5920,7 @@
         <v>342</v>
       </c>
       <c r="B384" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C384" s="3" t="s">
         <v>3</v>
@@ -5928,7 +5931,7 @@
         <v>342</v>
       </c>
       <c r="B385" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C385" s="3" t="s">
         <v>3</v>
@@ -5939,7 +5942,7 @@
         <v>342</v>
       </c>
       <c r="B386" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C386" s="3" t="s">
         <v>3</v>
@@ -5950,7 +5953,7 @@
         <v>342</v>
       </c>
       <c r="B387" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C387" s="3" t="s">
         <v>3</v>
@@ -5961,7 +5964,7 @@
         <v>342</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C388" s="3" t="s">
         <v>3</v>
@@ -5972,7 +5975,7 @@
         <v>342</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C389" s="3" t="s">
         <v>3</v>
@@ -5983,7 +5986,7 @@
         <v>342</v>
       </c>
       <c r="B390" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C390" s="3" t="s">
         <v>3</v>
@@ -5994,7 +5997,7 @@
         <v>342</v>
       </c>
       <c r="B391" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C391" s="3" t="s">
         <v>3</v>
@@ -6005,7 +6008,7 @@
         <v>342</v>
       </c>
       <c r="B392" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C392" s="3" t="s">
         <v>3</v>
@@ -6016,7 +6019,7 @@
         <v>342</v>
       </c>
       <c r="B393" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C393" s="3" t="s">
         <v>3</v>
@@ -6027,7 +6030,7 @@
         <v>342</v>
       </c>
       <c r="B394" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C394" s="3" t="s">
         <v>3</v>
@@ -6038,7 +6041,7 @@
         <v>342</v>
       </c>
       <c r="B395" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C395" s="3" t="s">
         <v>3</v>
@@ -6060,7 +6063,7 @@
         <v>342</v>
       </c>
       <c r="B397" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C397" s="3" t="s">
         <v>3</v>
@@ -6071,7 +6074,7 @@
         <v>342</v>
       </c>
       <c r="B398" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C398" s="3" t="s">
         <v>3</v>
@@ -6082,7 +6085,7 @@
         <v>342</v>
       </c>
       <c r="B399" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C399" s="3" t="s">
         <v>3</v>
@@ -6093,7 +6096,7 @@
         <v>342</v>
       </c>
       <c r="B400" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C400" s="3" t="s">
         <v>3</v>
@@ -6104,7 +6107,7 @@
         <v>342</v>
       </c>
       <c r="B401" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C401" s="3" t="s">
         <v>3</v>
@@ -6115,7 +6118,7 @@
         <v>342</v>
       </c>
       <c r="B402" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C402" s="3" t="s">
         <v>3</v>
@@ -6126,7 +6129,7 @@
         <v>342</v>
       </c>
       <c r="B403" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C403" s="3" t="s">
         <v>3</v>
@@ -6137,7 +6140,7 @@
         <v>342</v>
       </c>
       <c r="B404" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C404" s="3" t="s">
         <v>3</v>
@@ -6148,37 +6151,37 @@
         <v>342</v>
       </c>
       <c r="B405" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="C405" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" ht="21">
+      <c r="A406" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B406" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="C405" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="406" spans="1:3" ht="21">
-      <c r="B406" s="6"/>
-      <c r="C406" s="3"/>
+      <c r="C406" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="407" spans="1:3" ht="21">
       <c r="B407" s="6"/>
       <c r="C407" s="3"/>
     </row>
     <row r="408" spans="1:3" ht="21">
-      <c r="A408" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="B408" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="C408" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B408" s="6"/>
+      <c r="C408" s="3"/>
     </row>
     <row r="409" spans="1:3" ht="21">
       <c r="A409" s="7" t="s">
         <v>386</v>
       </c>
       <c r="B409" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C409" s="3" t="s">
         <v>3</v>
@@ -6189,7 +6192,7 @@
         <v>386</v>
       </c>
       <c r="B410" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C410" s="3" t="s">
         <v>3</v>
@@ -6200,7 +6203,7 @@
         <v>386</v>
       </c>
       <c r="B411" s="5" t="s">
-        <v>88</v>
+        <v>389</v>
       </c>
       <c r="C411" s="3" t="s">
         <v>3</v>
@@ -6211,7 +6214,7 @@
         <v>386</v>
       </c>
       <c r="B412" s="5" t="s">
-        <v>390</v>
+        <v>88</v>
       </c>
       <c r="C412" s="3" t="s">
         <v>3</v>
@@ -6222,37 +6225,37 @@
         <v>386</v>
       </c>
       <c r="B413" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C413" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" ht="21">
+      <c r="A414" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B414" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="C413" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="414" spans="1:3" ht="21">
-      <c r="B414" s="6"/>
-      <c r="C414" s="3"/>
+      <c r="C414" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="B415" s="6"/>
       <c r="C415" s="3"/>
     </row>
     <row r="416" spans="1:3" ht="21">
-      <c r="A416" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B416" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="C416" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B416" s="6"/>
+      <c r="C416" s="3"/>
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="4" t="s">
         <v>392</v>
       </c>
       <c r="B417" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C417" s="3" t="s">
         <v>3</v>
@@ -6263,7 +6266,7 @@
         <v>392</v>
       </c>
       <c r="B418" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C418" s="3" t="s">
         <v>3</v>
@@ -6274,7 +6277,7 @@
         <v>392</v>
       </c>
       <c r="B419" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C419" s="3" t="s">
         <v>3</v>
@@ -6285,7 +6288,7 @@
         <v>392</v>
       </c>
       <c r="B420" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C420" s="3" t="s">
         <v>3</v>
@@ -6296,7 +6299,7 @@
         <v>392</v>
       </c>
       <c r="B421" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C421" s="3" t="s">
         <v>3</v>
@@ -6307,7 +6310,7 @@
         <v>392</v>
       </c>
       <c r="B422" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C422" s="3" t="s">
         <v>3</v>
@@ -6318,7 +6321,7 @@
         <v>392</v>
       </c>
       <c r="B423" s="5" t="s">
-        <v>272</v>
+        <v>399</v>
       </c>
       <c r="C423" s="3" t="s">
         <v>3</v>
@@ -6329,7 +6332,7 @@
         <v>392</v>
       </c>
       <c r="B424" s="5" t="s">
-        <v>400</v>
+        <v>272</v>
       </c>
       <c r="C424" s="3" t="s">
         <v>3</v>
@@ -6340,7 +6343,7 @@
         <v>392</v>
       </c>
       <c r="B425" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C425" s="3" t="s">
         <v>3</v>
@@ -6351,7 +6354,7 @@
         <v>392</v>
       </c>
       <c r="B426" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C426" s="3" t="s">
         <v>3</v>
@@ -6362,7 +6365,7 @@
         <v>392</v>
       </c>
       <c r="B427" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C427" s="3" t="s">
         <v>3</v>
@@ -6373,7 +6376,7 @@
         <v>392</v>
       </c>
       <c r="B428" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C428" s="3" t="s">
         <v>3</v>
@@ -6384,7 +6387,7 @@
         <v>392</v>
       </c>
       <c r="B429" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C429" s="3" t="s">
         <v>3</v>
@@ -6395,7 +6398,7 @@
         <v>392</v>
       </c>
       <c r="B430" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C430" s="3" t="s">
         <v>3</v>
@@ -6406,7 +6409,7 @@
         <v>392</v>
       </c>
       <c r="B431" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C431" s="3" t="s">
         <v>3</v>
@@ -6417,7 +6420,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C432" s="3" t="s">
         <v>3</v>
@@ -6428,7 +6431,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C433" s="3" t="s">
         <v>3</v>
@@ -6439,7 +6442,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C434" s="3" t="s">
         <v>3</v>
@@ -6450,7 +6453,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C435" s="3" t="s">
         <v>3</v>
@@ -6461,7 +6464,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C436" s="3" t="s">
         <v>3</v>
@@ -6472,7 +6475,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C437" s="3" t="s">
         <v>3</v>
@@ -6483,7 +6486,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C438" s="3" t="s">
         <v>3</v>
@@ -6494,7 +6497,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C439" s="3" t="s">
         <v>3</v>
@@ -6505,7 +6508,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C440" s="3" t="s">
         <v>3</v>
@@ -6516,7 +6519,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C441" s="3" t="s">
         <v>3</v>
@@ -6527,7 +6530,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C442" s="3" t="s">
         <v>3</v>
@@ -6538,7 +6541,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C443" s="3" t="s">
         <v>3</v>
@@ -6549,7 +6552,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C444" s="3" t="s">
         <v>3</v>
@@ -6560,7 +6563,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C445" s="3" t="s">
         <v>3</v>
@@ -6571,7 +6574,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C446" s="3" t="s">
         <v>3</v>
@@ -6582,7 +6585,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C447" s="3" t="s">
         <v>3</v>
@@ -6593,7 +6596,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C448" s="3" t="s">
         <v>3</v>
@@ -6604,7 +6607,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C449" s="3" t="s">
         <v>3</v>
@@ -6615,7 +6618,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C450" s="3" t="s">
         <v>3</v>
@@ -6626,7 +6629,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C451" s="3" t="s">
         <v>3</v>
@@ -6637,7 +6640,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C452" s="3" t="s">
         <v>3</v>
@@ -6648,7 +6651,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C453" s="3" t="s">
         <v>3</v>
@@ -6659,7 +6662,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C454" s="3" t="s">
         <v>3</v>
@@ -6670,7 +6673,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C455" s="3" t="s">
         <v>3</v>
@@ -6681,7 +6684,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C456" s="3" t="s">
         <v>3</v>
@@ -6692,7 +6695,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C457" s="3" t="s">
         <v>3</v>
@@ -6703,7 +6706,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C458" s="3" t="s">
         <v>3</v>
@@ -6714,7 +6717,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C459" s="3" t="s">
         <v>3</v>
@@ -6725,7 +6728,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C460" s="3" t="s">
         <v>3</v>
@@ -6736,7 +6739,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C461" s="3" t="s">
         <v>3</v>
@@ -6747,7 +6750,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C462" s="3" t="s">
         <v>3</v>
@@ -6758,7 +6761,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C463" s="3" t="s">
         <v>3</v>
@@ -6769,7 +6772,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C464" s="3" t="s">
         <v>3</v>
@@ -6780,7 +6783,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C465" s="3" t="s">
         <v>3</v>
@@ -6791,7 +6794,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C466" s="3" t="s">
         <v>3</v>
@@ -6802,7 +6805,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C467" s="3" t="s">
         <v>3</v>
@@ -6813,7 +6816,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C468" s="3" t="s">
         <v>3</v>
@@ -6824,7 +6827,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C469" s="3" t="s">
         <v>3</v>
@@ -6835,7 +6838,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C470" s="3" t="s">
         <v>3</v>
@@ -6846,7 +6849,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C471" s="3" t="s">
         <v>3</v>
@@ -6857,7 +6860,7 @@
         <v>392</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C472" s="3" t="s">
         <v>3</v>
@@ -6868,7 +6871,7 @@
         <v>392</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C473" s="3" t="s">
         <v>3</v>
@@ -6879,7 +6882,7 @@
         <v>392</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C474" s="3" t="s">
         <v>3</v>
@@ -6890,38 +6893,38 @@
         <v>392</v>
       </c>
       <c r="B475" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="C475" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" ht="21">
+      <c r="A476" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B476" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="C475" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="476" spans="1:3" ht="21">
-      <c r="B476" s="6"/>
-      <c r="C476" s="3"/>
+      <c r="C476" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="477" spans="1:3" ht="21">
-      <c r="A477" s="7"/>
       <c r="B477" s="6"/>
       <c r="C477" s="3"/>
     </row>
     <row r="478" spans="1:3" ht="21">
-      <c r="A478" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B478" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="C478" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A478" s="7"/>
+      <c r="B478" s="6"/>
+      <c r="C478" s="3"/>
     </row>
     <row r="479" spans="1:3" ht="21">
       <c r="A479" s="4" t="s">
         <v>452</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C479" s="3" t="s">
         <v>3</v>
@@ -6932,7 +6935,7 @@
         <v>452</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C480" s="3" t="s">
         <v>3</v>
@@ -6943,7 +6946,7 @@
         <v>452</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C481" s="3" t="s">
         <v>3</v>
@@ -6954,7 +6957,7 @@
         <v>452</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C482" s="3" t="s">
         <v>3</v>
@@ -6965,7 +6968,7 @@
         <v>452</v>
       </c>
       <c r="B483" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C483" s="3" t="s">
         <v>3</v>
@@ -6976,7 +6979,7 @@
         <v>452</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C484" s="3" t="s">
         <v>3</v>
@@ -6987,7 +6990,7 @@
         <v>452</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C485" s="3" t="s">
         <v>3</v>
@@ -6998,7 +7001,7 @@
         <v>452</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C486" s="3" t="s">
         <v>3</v>
@@ -7009,9 +7012,20 @@
         <v>452</v>
       </c>
       <c r="B487" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="C487" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" ht="21">
+      <c r="A488" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B488" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="C487" s="3" t="s">
+      <c r="C488" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7175,293 +7189,293 @@
     <hyperlink ref="B178" r:id="rId156" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
     <hyperlink ref="B179" r:id="rId157" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
     <hyperlink ref="B180" r:id="rId158" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
-    <hyperlink ref="B183" r:id="rId159" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
-    <hyperlink ref="B184" r:id="rId160" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
-    <hyperlink ref="B185" r:id="rId161" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
-    <hyperlink ref="B186" r:id="rId162" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
-    <hyperlink ref="B187" r:id="rId163" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
-    <hyperlink ref="B188" r:id="rId164" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
-    <hyperlink ref="B189" r:id="rId165" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
-    <hyperlink ref="B190" r:id="rId166" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
-    <hyperlink ref="B191" r:id="rId167" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
-    <hyperlink ref="B192" r:id="rId168" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
-    <hyperlink ref="B193" r:id="rId169" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
-    <hyperlink ref="B194" r:id="rId170" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
-    <hyperlink ref="B195" r:id="rId171" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
-    <hyperlink ref="B196" r:id="rId172" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
-    <hyperlink ref="B197" r:id="rId173" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
-    <hyperlink ref="B198" r:id="rId174" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
-    <hyperlink ref="B199" r:id="rId175" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
-    <hyperlink ref="B200" r:id="rId176" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
-    <hyperlink ref="B201" r:id="rId177" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
-    <hyperlink ref="B202" r:id="rId178" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
-    <hyperlink ref="B203" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
-    <hyperlink ref="B204" r:id="rId180" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
-    <hyperlink ref="B205" r:id="rId181" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
-    <hyperlink ref="B206" r:id="rId182" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
-    <hyperlink ref="B207" r:id="rId183" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
-    <hyperlink ref="B208" r:id="rId184" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
-    <hyperlink ref="B209" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
-    <hyperlink ref="B210" r:id="rId186" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
-    <hyperlink ref="B211" r:id="rId187" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
-    <hyperlink ref="B212" r:id="rId188" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
-    <hyperlink ref="B213" r:id="rId189" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
-    <hyperlink ref="B214" r:id="rId190" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
-    <hyperlink ref="B215" r:id="rId191" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
-    <hyperlink ref="B216" r:id="rId192" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
-    <hyperlink ref="B217" r:id="rId193" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
-    <hyperlink ref="B220" r:id="rId194" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
-    <hyperlink ref="B221" r:id="rId195" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
-    <hyperlink ref="B222" r:id="rId196" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
-    <hyperlink ref="B223" r:id="rId197" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
-    <hyperlink ref="B224" r:id="rId198" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
-    <hyperlink ref="B225" r:id="rId199" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
-    <hyperlink ref="B226" r:id="rId200" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
-    <hyperlink ref="B227" r:id="rId201" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
-    <hyperlink ref="B228" r:id="rId202" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
-    <hyperlink ref="B229" r:id="rId203" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
-    <hyperlink ref="B230" r:id="rId204" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
-    <hyperlink ref="B231" r:id="rId205" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
-    <hyperlink ref="B232" r:id="rId206" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
-    <hyperlink ref="B233" r:id="rId207" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
-    <hyperlink ref="B234" r:id="rId208" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
-    <hyperlink ref="B235" r:id="rId209" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
-    <hyperlink ref="B236" r:id="rId210" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
-    <hyperlink ref="B237" r:id="rId211" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
-    <hyperlink ref="B238" r:id="rId212" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
-    <hyperlink ref="B239" r:id="rId213" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
-    <hyperlink ref="B240" r:id="rId214" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
-    <hyperlink ref="B241" r:id="rId215" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
-    <hyperlink ref="B244" r:id="rId216" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
-    <hyperlink ref="B245" r:id="rId217" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
-    <hyperlink ref="B246" r:id="rId218" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
-    <hyperlink ref="B247" r:id="rId219" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
-    <hyperlink ref="B248" r:id="rId220" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
-    <hyperlink ref="B249" r:id="rId221" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
-    <hyperlink ref="B250" r:id="rId222" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
-    <hyperlink ref="B251" r:id="rId223" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
-    <hyperlink ref="B252" r:id="rId224" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
-    <hyperlink ref="B253" r:id="rId225" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
-    <hyperlink ref="B254" r:id="rId226" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
-    <hyperlink ref="B255" r:id="rId227" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
-    <hyperlink ref="B256" r:id="rId228" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
-    <hyperlink ref="B257" r:id="rId229" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
-    <hyperlink ref="B258" r:id="rId230" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
-    <hyperlink ref="B259" r:id="rId231" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
-    <hyperlink ref="B260" r:id="rId232" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
-    <hyperlink ref="B261" r:id="rId233" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
-    <hyperlink ref="B262" r:id="rId234" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
-    <hyperlink ref="B263" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
-    <hyperlink ref="B264" r:id="rId236" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
-    <hyperlink ref="B265" r:id="rId237" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
-    <hyperlink ref="B266" r:id="rId238" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
-    <hyperlink ref="B267" r:id="rId239" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
-    <hyperlink ref="B268" r:id="rId240" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
-    <hyperlink ref="B269" r:id="rId241" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
-    <hyperlink ref="B270" r:id="rId242" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
-    <hyperlink ref="B271" r:id="rId243" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
-    <hyperlink ref="B272" r:id="rId244" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
-    <hyperlink ref="B273" r:id="rId245" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
-    <hyperlink ref="B274" r:id="rId246" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
-    <hyperlink ref="B275" r:id="rId247" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
-    <hyperlink ref="B276" r:id="rId248" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
-    <hyperlink ref="B277" r:id="rId249" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
-    <hyperlink ref="B278" r:id="rId250" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
-    <hyperlink ref="B281" r:id="rId251" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
-    <hyperlink ref="B282" r:id="rId252" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
-    <hyperlink ref="B283" r:id="rId253" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
-    <hyperlink ref="B284" r:id="rId254" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
-    <hyperlink ref="B285" r:id="rId255" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
-    <hyperlink ref="B286" r:id="rId256" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
-    <hyperlink ref="B287" r:id="rId257" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
-    <hyperlink ref="B288" r:id="rId258" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
-    <hyperlink ref="B289" r:id="rId259" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
-    <hyperlink ref="B290" r:id="rId260" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
-    <hyperlink ref="B291" r:id="rId261" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
-    <hyperlink ref="B292" r:id="rId262" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
-    <hyperlink ref="B293" r:id="rId263" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
-    <hyperlink ref="B294" r:id="rId264" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
-    <hyperlink ref="B295" r:id="rId265" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
-    <hyperlink ref="B296" r:id="rId266" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
-    <hyperlink ref="B297" r:id="rId267" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
-    <hyperlink ref="B298" r:id="rId268" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
-    <hyperlink ref="B299" r:id="rId269" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
-    <hyperlink ref="B302" r:id="rId270" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
-    <hyperlink ref="B303" r:id="rId271" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
-    <hyperlink ref="B304" r:id="rId272" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
-    <hyperlink ref="B305" r:id="rId273" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
-    <hyperlink ref="B306" r:id="rId274" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
-    <hyperlink ref="B307" r:id="rId275" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
-    <hyperlink ref="B308" r:id="rId276" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
-    <hyperlink ref="B309" r:id="rId277" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
-    <hyperlink ref="B310" r:id="rId278" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
-    <hyperlink ref="B311" r:id="rId279" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
-    <hyperlink ref="B312" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
-    <hyperlink ref="B313" r:id="rId281" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
-    <hyperlink ref="B314" r:id="rId282" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
-    <hyperlink ref="B315" r:id="rId283" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
-    <hyperlink ref="B316" r:id="rId284" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
-    <hyperlink ref="B317" r:id="rId285" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
-    <hyperlink ref="B318" r:id="rId286" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
-    <hyperlink ref="B319" r:id="rId287" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
-    <hyperlink ref="B320" r:id="rId288" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
-    <hyperlink ref="B321" r:id="rId289" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
-    <hyperlink ref="B322" r:id="rId290" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
-    <hyperlink ref="B323" r:id="rId291" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
-    <hyperlink ref="B324" r:id="rId292" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
-    <hyperlink ref="B325" r:id="rId293" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
-    <hyperlink ref="B326" r:id="rId294" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
-    <hyperlink ref="B327" r:id="rId295" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
-    <hyperlink ref="B328" r:id="rId296" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
-    <hyperlink ref="B329" r:id="rId297" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
-    <hyperlink ref="B330" r:id="rId298" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
-    <hyperlink ref="B331" r:id="rId299" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
-    <hyperlink ref="B332" r:id="rId300" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
-    <hyperlink ref="B333" r:id="rId301" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
-    <hyperlink ref="B334" r:id="rId302" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
-    <hyperlink ref="B335" r:id="rId303" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
-    <hyperlink ref="B336" r:id="rId304" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
-    <hyperlink ref="B337" r:id="rId305" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
-    <hyperlink ref="B338" r:id="rId306" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
-    <hyperlink ref="B339" r:id="rId307" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
-    <hyperlink ref="B342" r:id="rId308" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
-    <hyperlink ref="B343" r:id="rId309" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
-    <hyperlink ref="B344" r:id="rId310" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
-    <hyperlink ref="B345" r:id="rId311" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
-    <hyperlink ref="B346" r:id="rId312" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
-    <hyperlink ref="B347" r:id="rId313" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
-    <hyperlink ref="B348" r:id="rId314" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
-    <hyperlink ref="B349" r:id="rId315" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
-    <hyperlink ref="B350" r:id="rId316" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
-    <hyperlink ref="B351" r:id="rId317" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
-    <hyperlink ref="B352" r:id="rId318" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
-    <hyperlink ref="B353" r:id="rId319" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
-    <hyperlink ref="B354" r:id="rId320" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
-    <hyperlink ref="B355" r:id="rId321" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
-    <hyperlink ref="B356" r:id="rId322" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
-    <hyperlink ref="B357" r:id="rId323" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
-    <hyperlink ref="B358" r:id="rId324" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
-    <hyperlink ref="B359" r:id="rId325" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
-    <hyperlink ref="B363" r:id="rId326" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
-    <hyperlink ref="B364" r:id="rId327" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
-    <hyperlink ref="B365" r:id="rId328" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
-    <hyperlink ref="B366" r:id="rId329" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
-    <hyperlink ref="B367" r:id="rId330" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
-    <hyperlink ref="B368" r:id="rId331" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
-    <hyperlink ref="B369" r:id="rId332" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
-    <hyperlink ref="B370" r:id="rId333" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
-    <hyperlink ref="B371" r:id="rId334" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
-    <hyperlink ref="B372" r:id="rId335" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
-    <hyperlink ref="B373" r:id="rId336" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
-    <hyperlink ref="B374" r:id="rId337" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
-    <hyperlink ref="B375" r:id="rId338" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
-    <hyperlink ref="B376" r:id="rId339" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
-    <hyperlink ref="B377" r:id="rId340" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
-    <hyperlink ref="B378" r:id="rId341" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
-    <hyperlink ref="B379" r:id="rId342" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="B380" r:id="rId343" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="B381" r:id="rId344" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="B382" r:id="rId345" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="B383" r:id="rId346" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="B384" r:id="rId347" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="B385" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="B386" r:id="rId349" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="B387" r:id="rId350" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="B388" r:id="rId351" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="B389" r:id="rId352" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="B390" r:id="rId353" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="B391" r:id="rId354" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="B392" r:id="rId355" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="B393" r:id="rId356" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="B394" r:id="rId357" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="B395" r:id="rId358" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="B396" r:id="rId359" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="B397" r:id="rId360" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="B398" r:id="rId361" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="B399" r:id="rId362" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="B400" r:id="rId363" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="B402" r:id="rId364" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="B401" r:id="rId365" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="B403" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="B404" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="B405" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B408" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B409" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B410" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B411" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B412" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B413" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B416" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B417" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B418" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B419" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B420" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B421" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B422" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B423" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B424" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B425" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B426" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B427" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B428" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B429" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B430" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B431" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B432" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B433" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B434" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B435" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B436" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B437" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B438" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B439" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B440" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B441" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B442" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B443" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B444" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B445" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B446" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B447" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B448" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B449" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B450" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B451" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B452" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B453" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B454" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B455" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B457" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B456" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B458" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B459" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B460" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B461" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B462" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B463" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B464" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B465" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B466" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B467" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B468" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B475" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B474" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B473" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B472" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B471" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B470" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B469" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B478" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B479" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B480" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B481" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B482" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B483" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B484" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B487" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B485" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B486" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="B362" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
+    <hyperlink ref="B184" r:id="rId159" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
+    <hyperlink ref="B185" r:id="rId160" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
+    <hyperlink ref="B186" r:id="rId161" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
+    <hyperlink ref="B187" r:id="rId162" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
+    <hyperlink ref="B188" r:id="rId163" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
+    <hyperlink ref="B189" r:id="rId164" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
+    <hyperlink ref="B190" r:id="rId165" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
+    <hyperlink ref="B191" r:id="rId166" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
+    <hyperlink ref="B192" r:id="rId167" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
+    <hyperlink ref="B193" r:id="rId168" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
+    <hyperlink ref="B194" r:id="rId169" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
+    <hyperlink ref="B195" r:id="rId170" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
+    <hyperlink ref="B196" r:id="rId171" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
+    <hyperlink ref="B197" r:id="rId172" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
+    <hyperlink ref="B198" r:id="rId173" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
+    <hyperlink ref="B199" r:id="rId174" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
+    <hyperlink ref="B200" r:id="rId175" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
+    <hyperlink ref="B201" r:id="rId176" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
+    <hyperlink ref="B202" r:id="rId177" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
+    <hyperlink ref="B203" r:id="rId178" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
+    <hyperlink ref="B204" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
+    <hyperlink ref="B205" r:id="rId180" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
+    <hyperlink ref="B206" r:id="rId181" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
+    <hyperlink ref="B207" r:id="rId182" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
+    <hyperlink ref="B208" r:id="rId183" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
+    <hyperlink ref="B209" r:id="rId184" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
+    <hyperlink ref="B210" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
+    <hyperlink ref="B211" r:id="rId186" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
+    <hyperlink ref="B212" r:id="rId187" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
+    <hyperlink ref="B213" r:id="rId188" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
+    <hyperlink ref="B214" r:id="rId189" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
+    <hyperlink ref="B215" r:id="rId190" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
+    <hyperlink ref="B216" r:id="rId191" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
+    <hyperlink ref="B217" r:id="rId192" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
+    <hyperlink ref="B218" r:id="rId193" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
+    <hyperlink ref="B221" r:id="rId194" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
+    <hyperlink ref="B222" r:id="rId195" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
+    <hyperlink ref="B223" r:id="rId196" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
+    <hyperlink ref="B224" r:id="rId197" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
+    <hyperlink ref="B225" r:id="rId198" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
+    <hyperlink ref="B226" r:id="rId199" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
+    <hyperlink ref="B227" r:id="rId200" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
+    <hyperlink ref="B228" r:id="rId201" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
+    <hyperlink ref="B229" r:id="rId202" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
+    <hyperlink ref="B230" r:id="rId203" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
+    <hyperlink ref="B231" r:id="rId204" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
+    <hyperlink ref="B232" r:id="rId205" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
+    <hyperlink ref="B233" r:id="rId206" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
+    <hyperlink ref="B234" r:id="rId207" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
+    <hyperlink ref="B235" r:id="rId208" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
+    <hyperlink ref="B236" r:id="rId209" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
+    <hyperlink ref="B237" r:id="rId210" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
+    <hyperlink ref="B238" r:id="rId211" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
+    <hyperlink ref="B239" r:id="rId212" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
+    <hyperlink ref="B240" r:id="rId213" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
+    <hyperlink ref="B241" r:id="rId214" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
+    <hyperlink ref="B242" r:id="rId215" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
+    <hyperlink ref="B245" r:id="rId216" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
+    <hyperlink ref="B246" r:id="rId217" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
+    <hyperlink ref="B247" r:id="rId218" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
+    <hyperlink ref="B248" r:id="rId219" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
+    <hyperlink ref="B249" r:id="rId220" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
+    <hyperlink ref="B250" r:id="rId221" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
+    <hyperlink ref="B251" r:id="rId222" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
+    <hyperlink ref="B252" r:id="rId223" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
+    <hyperlink ref="B253" r:id="rId224" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
+    <hyperlink ref="B254" r:id="rId225" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
+    <hyperlink ref="B255" r:id="rId226" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
+    <hyperlink ref="B256" r:id="rId227" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
+    <hyperlink ref="B257" r:id="rId228" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
+    <hyperlink ref="B258" r:id="rId229" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
+    <hyperlink ref="B259" r:id="rId230" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
+    <hyperlink ref="B260" r:id="rId231" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
+    <hyperlink ref="B261" r:id="rId232" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
+    <hyperlink ref="B262" r:id="rId233" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
+    <hyperlink ref="B263" r:id="rId234" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
+    <hyperlink ref="B264" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
+    <hyperlink ref="B265" r:id="rId236" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
+    <hyperlink ref="B266" r:id="rId237" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
+    <hyperlink ref="B267" r:id="rId238" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
+    <hyperlink ref="B268" r:id="rId239" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
+    <hyperlink ref="B269" r:id="rId240" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
+    <hyperlink ref="B270" r:id="rId241" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
+    <hyperlink ref="B271" r:id="rId242" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
+    <hyperlink ref="B272" r:id="rId243" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
+    <hyperlink ref="B273" r:id="rId244" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
+    <hyperlink ref="B274" r:id="rId245" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
+    <hyperlink ref="B275" r:id="rId246" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
+    <hyperlink ref="B276" r:id="rId247" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
+    <hyperlink ref="B277" r:id="rId248" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
+    <hyperlink ref="B278" r:id="rId249" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
+    <hyperlink ref="B279" r:id="rId250" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
+    <hyperlink ref="B282" r:id="rId251" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
+    <hyperlink ref="B283" r:id="rId252" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
+    <hyperlink ref="B284" r:id="rId253" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
+    <hyperlink ref="B285" r:id="rId254" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
+    <hyperlink ref="B286" r:id="rId255" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
+    <hyperlink ref="B287" r:id="rId256" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
+    <hyperlink ref="B288" r:id="rId257" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
+    <hyperlink ref="B289" r:id="rId258" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
+    <hyperlink ref="B290" r:id="rId259" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
+    <hyperlink ref="B291" r:id="rId260" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
+    <hyperlink ref="B292" r:id="rId261" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
+    <hyperlink ref="B293" r:id="rId262" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
+    <hyperlink ref="B294" r:id="rId263" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
+    <hyperlink ref="B295" r:id="rId264" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
+    <hyperlink ref="B296" r:id="rId265" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
+    <hyperlink ref="B297" r:id="rId266" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
+    <hyperlink ref="B298" r:id="rId267" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
+    <hyperlink ref="B299" r:id="rId268" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="B300" r:id="rId269" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
+    <hyperlink ref="B303" r:id="rId270" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
+    <hyperlink ref="B304" r:id="rId271" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
+    <hyperlink ref="B305" r:id="rId272" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
+    <hyperlink ref="B306" r:id="rId273" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
+    <hyperlink ref="B307" r:id="rId274" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
+    <hyperlink ref="B308" r:id="rId275" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
+    <hyperlink ref="B309" r:id="rId276" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
+    <hyperlink ref="B310" r:id="rId277" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
+    <hyperlink ref="B311" r:id="rId278" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
+    <hyperlink ref="B312" r:id="rId279" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
+    <hyperlink ref="B313" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
+    <hyperlink ref="B314" r:id="rId281" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
+    <hyperlink ref="B315" r:id="rId282" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
+    <hyperlink ref="B316" r:id="rId283" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
+    <hyperlink ref="B317" r:id="rId284" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
+    <hyperlink ref="B318" r:id="rId285" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
+    <hyperlink ref="B319" r:id="rId286" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
+    <hyperlink ref="B320" r:id="rId287" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
+    <hyperlink ref="B321" r:id="rId288" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
+    <hyperlink ref="B322" r:id="rId289" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
+    <hyperlink ref="B323" r:id="rId290" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
+    <hyperlink ref="B324" r:id="rId291" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
+    <hyperlink ref="B325" r:id="rId292" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
+    <hyperlink ref="B326" r:id="rId293" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
+    <hyperlink ref="B327" r:id="rId294" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
+    <hyperlink ref="B328" r:id="rId295" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
+    <hyperlink ref="B329" r:id="rId296" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
+    <hyperlink ref="B330" r:id="rId297" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
+    <hyperlink ref="B331" r:id="rId298" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
+    <hyperlink ref="B332" r:id="rId299" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
+    <hyperlink ref="B333" r:id="rId300" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
+    <hyperlink ref="B334" r:id="rId301" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
+    <hyperlink ref="B335" r:id="rId302" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
+    <hyperlink ref="B336" r:id="rId303" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
+    <hyperlink ref="B337" r:id="rId304" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
+    <hyperlink ref="B338" r:id="rId305" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
+    <hyperlink ref="B339" r:id="rId306" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
+    <hyperlink ref="B340" r:id="rId307" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
+    <hyperlink ref="B343" r:id="rId308" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
+    <hyperlink ref="B344" r:id="rId309" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
+    <hyperlink ref="B345" r:id="rId310" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
+    <hyperlink ref="B346" r:id="rId311" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
+    <hyperlink ref="B347" r:id="rId312" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
+    <hyperlink ref="B348" r:id="rId313" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
+    <hyperlink ref="B349" r:id="rId314" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
+    <hyperlink ref="B350" r:id="rId315" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
+    <hyperlink ref="B351" r:id="rId316" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
+    <hyperlink ref="B352" r:id="rId317" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
+    <hyperlink ref="B353" r:id="rId318" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
+    <hyperlink ref="B354" r:id="rId319" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
+    <hyperlink ref="B355" r:id="rId320" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
+    <hyperlink ref="B356" r:id="rId321" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
+    <hyperlink ref="B357" r:id="rId322" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
+    <hyperlink ref="B358" r:id="rId323" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
+    <hyperlink ref="B359" r:id="rId324" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
+    <hyperlink ref="B360" r:id="rId325" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
+    <hyperlink ref="B364" r:id="rId326" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
+    <hyperlink ref="B365" r:id="rId327" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
+    <hyperlink ref="B366" r:id="rId328" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
+    <hyperlink ref="B367" r:id="rId329" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
+    <hyperlink ref="B368" r:id="rId330" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
+    <hyperlink ref="B369" r:id="rId331" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
+    <hyperlink ref="B370" r:id="rId332" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
+    <hyperlink ref="B371" r:id="rId333" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
+    <hyperlink ref="B372" r:id="rId334" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
+    <hyperlink ref="B373" r:id="rId335" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
+    <hyperlink ref="B374" r:id="rId336" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
+    <hyperlink ref="B375" r:id="rId337" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
+    <hyperlink ref="B376" r:id="rId338" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
+    <hyperlink ref="B377" r:id="rId339" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
+    <hyperlink ref="B378" r:id="rId340" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
+    <hyperlink ref="B379" r:id="rId341" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
+    <hyperlink ref="B380" r:id="rId342" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
+    <hyperlink ref="B381" r:id="rId343" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
+    <hyperlink ref="B382" r:id="rId344" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
+    <hyperlink ref="B383" r:id="rId345" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
+    <hyperlink ref="B384" r:id="rId346" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
+    <hyperlink ref="B385" r:id="rId347" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
+    <hyperlink ref="B386" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="B387" r:id="rId349" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="B388" r:id="rId350" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="B389" r:id="rId351" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="B390" r:id="rId352" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="B391" r:id="rId353" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="B392" r:id="rId354" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="B393" r:id="rId355" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="B394" r:id="rId356" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="B395" r:id="rId357" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="B396" r:id="rId358" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="B397" r:id="rId359" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="B398" r:id="rId360" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="B399" r:id="rId361" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="B400" r:id="rId362" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="B401" r:id="rId363" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="B403" r:id="rId364" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="B402" r:id="rId365" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="B404" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="B405" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="B406" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="B409" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B410" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B411" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B412" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B413" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B414" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B417" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B418" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B419" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B420" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B421" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B422" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B423" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B424" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B425" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B426" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B427" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B428" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B429" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B430" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B431" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B432" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B433" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B434" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B435" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B436" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B437" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B438" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B439" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B440" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B441" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B442" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B443" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B444" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B445" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B446" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B447" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B448" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B449" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B450" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B451" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B452" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B453" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B454" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B455" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B456" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B458" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B457" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B459" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B460" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B461" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B462" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B463" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B464" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B465" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B466" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B467" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B468" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B469" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B476" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B475" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B474" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B473" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B472" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B471" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B470" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B479" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B480" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B481" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B482" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B483" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B484" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B485" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B488" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B486" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B487" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B363" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added and Solved "Merge two Sorted Linked List" from Striver in 450 DSA Sheet
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1316eb900441c6a3/Desktop/450 DSA and 30 Day Striver/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{B942E4A6-CC2E-45D9-BD08-117F0B38A8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDCBD13C-2C70-4830-8851-F19ECDD29B30}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A54E19-0773-4C25-8DF1-C83D88878193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="475">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1447,6 +1447,9 @@
   </si>
   <si>
     <t>Find Middle of the Linked List</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Linked List</t>
   </si>
 </sst>
 </file>
@@ -1884,10 +1887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:C488"/>
+  <dimension ref="A1:C489"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A168" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+      <selection activeCell="C183" sqref="C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3793,27 +3796,27 @@
         <v>465</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="21">
-      <c r="B183" s="6"/>
-      <c r="C183" s="3"/>
+    <row r="182" spans="1:3" ht="19.5">
+      <c r="A182" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B182" t="s">
+        <v>474</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="184" spans="1:3" ht="21">
-      <c r="A184" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B184" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B184" s="6"/>
+      <c r="C184" s="3"/>
     </row>
     <row r="185" spans="1:3" ht="21">
       <c r="A185" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>3</v>
@@ -3824,7 +3827,7 @@
         <v>170</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>3</v>
@@ -3835,7 +3838,7 @@
         <v>170</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>3</v>
@@ -3846,7 +3849,7 @@
         <v>170</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>3</v>
@@ -3857,7 +3860,7 @@
         <v>170</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>3</v>
@@ -3868,7 +3871,7 @@
         <v>170</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>3</v>
@@ -3879,7 +3882,7 @@
         <v>170</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>3</v>
@@ -3890,7 +3893,7 @@
         <v>170</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>3</v>
@@ -3901,7 +3904,7 @@
         <v>170</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>3</v>
@@ -3912,7 +3915,7 @@
         <v>170</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>3</v>
@@ -3923,7 +3926,7 @@
         <v>170</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>3</v>
@@ -3934,7 +3937,7 @@
         <v>170</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>3</v>
@@ -3945,7 +3948,7 @@
         <v>170</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>3</v>
@@ -3956,7 +3959,7 @@
         <v>170</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>3</v>
@@ -3967,7 +3970,7 @@
         <v>170</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>3</v>
@@ -3978,7 +3981,7 @@
         <v>170</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>3</v>
@@ -3989,7 +3992,7 @@
         <v>170</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>3</v>
@@ -4000,7 +4003,7 @@
         <v>170</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C202" s="3" t="s">
         <v>3</v>
@@ -4011,7 +4014,7 @@
         <v>170</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>3</v>
@@ -4022,7 +4025,7 @@
         <v>170</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>3</v>
@@ -4033,7 +4036,7 @@
         <v>170</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>3</v>
@@ -4044,7 +4047,7 @@
         <v>170</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>3</v>
@@ -4055,7 +4058,7 @@
         <v>170</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>3</v>
@@ -4066,7 +4069,7 @@
         <v>170</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>3</v>
@@ -4077,7 +4080,7 @@
         <v>170</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>3</v>
@@ -4088,7 +4091,7 @@
         <v>170</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>3</v>
@@ -4099,7 +4102,7 @@
         <v>170</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>3</v>
@@ -4110,7 +4113,7 @@
         <v>170</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>3</v>
@@ -4121,7 +4124,7 @@
         <v>170</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>3</v>
@@ -4132,7 +4135,7 @@
         <v>170</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>3</v>
@@ -4143,7 +4146,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>3</v>
@@ -4154,7 +4157,7 @@
         <v>170</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>3</v>
@@ -4165,7 +4168,7 @@
         <v>170</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>3</v>
@@ -4176,16 +4179,22 @@
         <v>170</v>
       </c>
       <c r="B218" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="21">
+      <c r="A219" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B219" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C218" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="21">
-      <c r="A219" s="7"/>
-      <c r="B219" s="6"/>
-      <c r="C219" s="3"/>
+      <c r="C219" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="220" spans="1:3" ht="21">
       <c r="A220" s="7"/>
@@ -4193,22 +4202,16 @@
       <c r="C220" s="3"/>
     </row>
     <row r="221" spans="1:3" ht="21">
-      <c r="A221" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B221" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C221" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A221" s="7"/>
+      <c r="B221" s="6"/>
+      <c r="C221" s="3"/>
     </row>
     <row r="222" spans="1:3" ht="21">
       <c r="A222" s="4" t="s">
         <v>206</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>3</v>
@@ -4219,7 +4222,7 @@
         <v>206</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>3</v>
@@ -4230,7 +4233,7 @@
         <v>206</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>3</v>
@@ -4241,7 +4244,7 @@
         <v>206</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>3</v>
@@ -4252,7 +4255,7 @@
         <v>206</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>3</v>
@@ -4262,8 +4265,8 @@
       <c r="A227" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B227" s="8" t="s">
-        <v>213</v>
+      <c r="B227" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>3</v>
@@ -4273,8 +4276,8 @@
       <c r="A228" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B228" s="5" t="s">
-        <v>214</v>
+      <c r="B228" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="C228" s="3" t="s">
         <v>3</v>
@@ -4285,7 +4288,7 @@
         <v>206</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>3</v>
@@ -4296,7 +4299,7 @@
         <v>206</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>3</v>
@@ -4307,7 +4310,7 @@
         <v>206</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>3</v>
@@ -4318,7 +4321,7 @@
         <v>206</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>3</v>
@@ -4329,7 +4332,7 @@
         <v>206</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>3</v>
@@ -4340,7 +4343,7 @@
         <v>206</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>3</v>
@@ -4351,7 +4354,7 @@
         <v>206</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>3</v>
@@ -4362,7 +4365,7 @@
         <v>206</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>3</v>
@@ -4373,7 +4376,7 @@
         <v>206</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>3</v>
@@ -4384,7 +4387,7 @@
         <v>206</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>3</v>
@@ -4395,7 +4398,7 @@
         <v>206</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>3</v>
@@ -4406,7 +4409,7 @@
         <v>206</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>3</v>
@@ -4417,7 +4420,7 @@
         <v>206</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C241" s="3" t="s">
         <v>3</v>
@@ -4428,37 +4431,37 @@
         <v>206</v>
       </c>
       <c r="B242" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" ht="21">
+      <c r="A243" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B243" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C242" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" ht="21">
-      <c r="B243" s="6"/>
-      <c r="C243" s="3"/>
+      <c r="C243" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="244" spans="1:3" ht="21">
       <c r="B244" s="6"/>
       <c r="C244" s="3"/>
     </row>
     <row r="245" spans="1:3" ht="21">
-      <c r="A245" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B245" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="C245" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B245" s="6"/>
+      <c r="C245" s="3"/>
     </row>
     <row r="246" spans="1:3" ht="21">
       <c r="A246" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>3</v>
@@ -4469,7 +4472,7 @@
         <v>229</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>3</v>
@@ -4480,7 +4483,7 @@
         <v>229</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>3</v>
@@ -4491,7 +4494,7 @@
         <v>229</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>3</v>
@@ -4502,7 +4505,7 @@
         <v>229</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C250" s="3" t="s">
         <v>3</v>
@@ -4513,7 +4516,7 @@
         <v>229</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C251" s="3" t="s">
         <v>3</v>
@@ -4524,7 +4527,7 @@
         <v>229</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C252" s="3" t="s">
         <v>3</v>
@@ -4535,7 +4538,7 @@
         <v>229</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C253" s="3" t="s">
         <v>3</v>
@@ -4546,7 +4549,7 @@
         <v>229</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>3</v>
@@ -4557,7 +4560,7 @@
         <v>229</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>3</v>
@@ -4568,7 +4571,7 @@
         <v>229</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>3</v>
@@ -4579,7 +4582,7 @@
         <v>229</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>3</v>
@@ -4590,7 +4593,7 @@
         <v>229</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>3</v>
@@ -4601,7 +4604,7 @@
         <v>229</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>3</v>
@@ -4612,7 +4615,7 @@
         <v>229</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>3</v>
@@ -4623,7 +4626,7 @@
         <v>229</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>3</v>
@@ -4634,7 +4637,7 @@
         <v>229</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C262" s="3" t="s">
         <v>3</v>
@@ -4645,7 +4648,7 @@
         <v>229</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>3</v>
@@ -4656,7 +4659,7 @@
         <v>229</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C264" s="3" t="s">
         <v>3</v>
@@ -4667,7 +4670,7 @@
         <v>229</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>3</v>
@@ -4678,7 +4681,7 @@
         <v>229</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>3</v>
@@ -4689,7 +4692,7 @@
         <v>229</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>3</v>
@@ -4700,7 +4703,7 @@
         <v>229</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C268" s="3" t="s">
         <v>3</v>
@@ -4711,7 +4714,7 @@
         <v>229</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C269" s="3" t="s">
         <v>3</v>
@@ -4722,7 +4725,7 @@
         <v>229</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C270" s="3" t="s">
         <v>3</v>
@@ -4733,7 +4736,7 @@
         <v>229</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C271" s="3" t="s">
         <v>3</v>
@@ -4744,7 +4747,7 @@
         <v>229</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>3</v>
@@ -4755,7 +4758,7 @@
         <v>229</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>3</v>
@@ -4766,7 +4769,7 @@
         <v>229</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C274" s="3" t="s">
         <v>3</v>
@@ -4777,7 +4780,7 @@
         <v>229</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>3</v>
@@ -4788,7 +4791,7 @@
         <v>229</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C276" s="3" t="s">
         <v>3</v>
@@ -4799,7 +4802,7 @@
         <v>229</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C277" s="3" t="s">
         <v>3</v>
@@ -4810,7 +4813,7 @@
         <v>229</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>86</v>
+        <v>262</v>
       </c>
       <c r="C278" s="3" t="s">
         <v>3</v>
@@ -4821,37 +4824,37 @@
         <v>229</v>
       </c>
       <c r="B279" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C279" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" ht="21">
+      <c r="A280" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B280" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C279" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" ht="21">
-      <c r="B280" s="6"/>
-      <c r="C280" s="3"/>
+      <c r="C280" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="281" spans="1:3" ht="21">
       <c r="B281" s="6"/>
       <c r="C281" s="3"/>
     </row>
     <row r="282" spans="1:3" ht="21">
-      <c r="A282" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B282" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C282" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B282" s="6"/>
+      <c r="C282" s="3"/>
     </row>
     <row r="283" spans="1:3" ht="21">
       <c r="A283" s="4" t="s">
         <v>264</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>3</v>
@@ -4862,7 +4865,7 @@
         <v>264</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>3</v>
@@ -4873,7 +4876,7 @@
         <v>264</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C285" s="3" t="s">
         <v>3</v>
@@ -4884,7 +4887,7 @@
         <v>264</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C286" s="3" t="s">
         <v>3</v>
@@ -4895,7 +4898,7 @@
         <v>264</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C287" s="3" t="s">
         <v>3</v>
@@ -4906,7 +4909,7 @@
         <v>264</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>3</v>
@@ -4917,7 +4920,7 @@
         <v>264</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C289" s="3" t="s">
         <v>3</v>
@@ -4928,7 +4931,7 @@
         <v>264</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C290" s="3" t="s">
         <v>3</v>
@@ -4939,7 +4942,7 @@
         <v>264</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>3</v>
@@ -4950,7 +4953,7 @@
         <v>264</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>3</v>
@@ -4961,7 +4964,7 @@
         <v>264</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C293" s="3" t="s">
         <v>3</v>
@@ -4972,7 +4975,7 @@
         <v>264</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C294" s="3" t="s">
         <v>3</v>
@@ -4983,7 +4986,7 @@
         <v>264</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C295" s="3" t="s">
         <v>3</v>
@@ -4994,7 +4997,7 @@
         <v>264</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C296" s="3" t="s">
         <v>3</v>
@@ -5005,7 +5008,7 @@
         <v>264</v>
       </c>
       <c r="B297" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C297" s="3" t="s">
         <v>3</v>
@@ -5016,7 +5019,7 @@
         <v>264</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C298" s="3" t="s">
         <v>3</v>
@@ -5027,7 +5030,7 @@
         <v>264</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C299" s="3" t="s">
         <v>3</v>
@@ -5038,37 +5041,37 @@
         <v>264</v>
       </c>
       <c r="B300" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C300" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" ht="21">
+      <c r="A301" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B301" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C300" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" ht="21">
-      <c r="B301" s="6"/>
-      <c r="C301" s="3"/>
+      <c r="C301" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="302" spans="1:3" ht="21">
       <c r="B302" s="6"/>
       <c r="C302" s="3"/>
     </row>
     <row r="303" spans="1:3" ht="21">
-      <c r="A303" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B303" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="C303" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B303" s="6"/>
+      <c r="C303" s="3"/>
     </row>
     <row r="304" spans="1:3" ht="21">
       <c r="A304" s="4" t="s">
         <v>284</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C304" s="3" t="s">
         <v>3</v>
@@ -5079,7 +5082,7 @@
         <v>284</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C305" s="3" t="s">
         <v>3</v>
@@ -5090,7 +5093,7 @@
         <v>284</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C306" s="3" t="s">
         <v>3</v>
@@ -5101,7 +5104,7 @@
         <v>284</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C307" s="3" t="s">
         <v>3</v>
@@ -5112,7 +5115,7 @@
         <v>284</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C308" s="3" t="s">
         <v>3</v>
@@ -5123,7 +5126,7 @@
         <v>284</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C309" s="3" t="s">
         <v>3</v>
@@ -5134,7 +5137,7 @@
         <v>284</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C310" s="3" t="s">
         <v>3</v>
@@ -5145,7 +5148,7 @@
         <v>284</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C311" s="3" t="s">
         <v>3</v>
@@ -5156,7 +5159,7 @@
         <v>284</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>3</v>
@@ -5167,7 +5170,7 @@
         <v>284</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C313" s="3" t="s">
         <v>3</v>
@@ -5178,7 +5181,7 @@
         <v>284</v>
       </c>
       <c r="B314" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>3</v>
@@ -5189,7 +5192,7 @@
         <v>284</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>3</v>
@@ -5199,8 +5202,8 @@
       <c r="A316" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B316" s="8" t="s">
-        <v>298</v>
+      <c r="B316" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="C316" s="3" t="s">
         <v>3</v>
@@ -5210,8 +5213,8 @@
       <c r="A317" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B317" s="5" t="s">
-        <v>299</v>
+      <c r="B317" s="8" t="s">
+        <v>298</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>3</v>
@@ -5222,7 +5225,7 @@
         <v>284</v>
       </c>
       <c r="B318" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>3</v>
@@ -5233,7 +5236,7 @@
         <v>284</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>3</v>
@@ -5244,7 +5247,7 @@
         <v>284</v>
       </c>
       <c r="B320" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C320" s="3" t="s">
         <v>3</v>
@@ -5255,7 +5258,7 @@
         <v>284</v>
       </c>
       <c r="B321" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C321" s="3" t="s">
         <v>3</v>
@@ -5266,7 +5269,7 @@
         <v>284</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C322" s="3" t="s">
         <v>3</v>
@@ -5277,7 +5280,7 @@
         <v>284</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C323" s="3" t="s">
         <v>3</v>
@@ -5288,7 +5291,7 @@
         <v>284</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C324" s="3" t="s">
         <v>3</v>
@@ -5299,7 +5302,7 @@
         <v>284</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C325" s="3" t="s">
         <v>3</v>
@@ -5310,7 +5313,7 @@
         <v>284</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>3</v>
@@ -5321,7 +5324,7 @@
         <v>284</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C327" s="3" t="s">
         <v>3</v>
@@ -5332,7 +5335,7 @@
         <v>284</v>
       </c>
       <c r="B328" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>3</v>
@@ -5343,7 +5346,7 @@
         <v>284</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C329" s="3" t="s">
         <v>3</v>
@@ -5354,7 +5357,7 @@
         <v>284</v>
       </c>
       <c r="B330" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C330" s="3" t="s">
         <v>3</v>
@@ -5365,7 +5368,7 @@
         <v>284</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C331" s="3" t="s">
         <v>3</v>
@@ -5376,7 +5379,7 @@
         <v>284</v>
       </c>
       <c r="B332" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>3</v>
@@ -5387,7 +5390,7 @@
         <v>284</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C333" s="3" t="s">
         <v>3</v>
@@ -5398,7 +5401,7 @@
         <v>284</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C334" s="3" t="s">
         <v>3</v>
@@ -5409,7 +5412,7 @@
         <v>284</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C335" s="3" t="s">
         <v>3</v>
@@ -5420,7 +5423,7 @@
         <v>284</v>
       </c>
       <c r="B336" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C336" s="3" t="s">
         <v>3</v>
@@ -5431,7 +5434,7 @@
         <v>284</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C337" s="3" t="s">
         <v>3</v>
@@ -5442,7 +5445,7 @@
         <v>284</v>
       </c>
       <c r="B338" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C338" s="3" t="s">
         <v>3</v>
@@ -5453,7 +5456,7 @@
         <v>284</v>
       </c>
       <c r="B339" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C339" s="3" t="s">
         <v>3</v>
@@ -5464,37 +5467,37 @@
         <v>284</v>
       </c>
       <c r="B340" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C340" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" ht="21">
+      <c r="A341" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B341" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="C340" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="341" spans="1:3" ht="21">
-      <c r="B341" s="6"/>
-      <c r="C341" s="3"/>
+      <c r="C341" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="342" spans="1:3" ht="21">
       <c r="B342" s="6"/>
       <c r="C342" s="3"/>
     </row>
     <row r="343" spans="1:3" ht="21">
-      <c r="A343" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B343" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="C343" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B343" s="6"/>
+      <c r="C343" s="3"/>
     </row>
     <row r="344" spans="1:3" ht="21">
       <c r="A344" s="7" t="s">
         <v>323</v>
       </c>
       <c r="B344" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>3</v>
@@ -5505,7 +5508,7 @@
         <v>323</v>
       </c>
       <c r="B345" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C345" s="3" t="s">
         <v>3</v>
@@ -5516,7 +5519,7 @@
         <v>323</v>
       </c>
       <c r="B346" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C346" s="3" t="s">
         <v>3</v>
@@ -5527,7 +5530,7 @@
         <v>323</v>
       </c>
       <c r="B347" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C347" s="3" t="s">
         <v>3</v>
@@ -5538,7 +5541,7 @@
         <v>323</v>
       </c>
       <c r="B348" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C348" s="3" t="s">
         <v>3</v>
@@ -5549,7 +5552,7 @@
         <v>323</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>3</v>
@@ -5560,7 +5563,7 @@
         <v>323</v>
       </c>
       <c r="B350" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C350" s="3" t="s">
         <v>3</v>
@@ -5570,8 +5573,8 @@
       <c r="A351" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B351" s="8" t="s">
-        <v>332</v>
+      <c r="B351" s="5" t="s">
+        <v>331</v>
       </c>
       <c r="C351" s="3" t="s">
         <v>3</v>
@@ -5581,8 +5584,8 @@
       <c r="A352" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B352" s="5" t="s">
-        <v>333</v>
+      <c r="B352" s="8" t="s">
+        <v>332</v>
       </c>
       <c r="C352" s="3" t="s">
         <v>3</v>
@@ -5593,7 +5596,7 @@
         <v>323</v>
       </c>
       <c r="B353" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C353" s="3" t="s">
         <v>3</v>
@@ -5604,7 +5607,7 @@
         <v>323</v>
       </c>
       <c r="B354" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C354" s="3" t="s">
         <v>3</v>
@@ -5615,7 +5618,7 @@
         <v>323</v>
       </c>
       <c r="B355" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C355" s="3" t="s">
         <v>3</v>
@@ -5626,7 +5629,7 @@
         <v>323</v>
       </c>
       <c r="B356" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>3</v>
@@ -5637,7 +5640,7 @@
         <v>323</v>
       </c>
       <c r="B357" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C357" s="3" t="s">
         <v>3</v>
@@ -5648,7 +5651,7 @@
         <v>323</v>
       </c>
       <c r="B358" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C358" s="3" t="s">
         <v>3</v>
@@ -5659,7 +5662,7 @@
         <v>323</v>
       </c>
       <c r="B359" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C359" s="3" t="s">
         <v>3</v>
@@ -5670,37 +5673,37 @@
         <v>323</v>
       </c>
       <c r="B360" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C360" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" ht="21">
+      <c r="A361" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B361" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="C360" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="361" spans="1:3" ht="21">
-      <c r="B361" s="6"/>
-      <c r="C361" s="3"/>
+      <c r="C361" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="B362" s="6"/>
       <c r="C362" s="3"/>
     </row>
     <row r="363" spans="1:3" ht="21">
-      <c r="A363" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B363" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="C363" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B363" s="6"/>
+      <c r="C363" s="3"/>
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="7" t="s">
         <v>342</v>
       </c>
       <c r="B364" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C364" s="3" t="s">
         <v>3</v>
@@ -5711,7 +5714,7 @@
         <v>342</v>
       </c>
       <c r="B365" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C365" s="3" t="s">
         <v>3</v>
@@ -5722,7 +5725,7 @@
         <v>342</v>
       </c>
       <c r="B366" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C366" s="3" t="s">
         <v>3</v>
@@ -5733,7 +5736,7 @@
         <v>342</v>
       </c>
       <c r="B367" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C367" s="3" t="s">
         <v>3</v>
@@ -5744,7 +5747,7 @@
         <v>342</v>
       </c>
       <c r="B368" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C368" s="3" t="s">
         <v>3</v>
@@ -5755,7 +5758,7 @@
         <v>342</v>
       </c>
       <c r="B369" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C369" s="3" t="s">
         <v>3</v>
@@ -5766,7 +5769,7 @@
         <v>342</v>
       </c>
       <c r="B370" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C370" s="3" t="s">
         <v>3</v>
@@ -5777,7 +5780,7 @@
         <v>342</v>
       </c>
       <c r="B371" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C371" s="3" t="s">
         <v>3</v>
@@ -5788,7 +5791,7 @@
         <v>342</v>
       </c>
       <c r="B372" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C372" s="3" t="s">
         <v>3</v>
@@ -5799,7 +5802,7 @@
         <v>342</v>
       </c>
       <c r="B373" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>3</v>
@@ -5810,7 +5813,7 @@
         <v>342</v>
       </c>
       <c r="B374" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>3</v>
@@ -5821,7 +5824,7 @@
         <v>342</v>
       </c>
       <c r="B375" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>3</v>
@@ -5832,7 +5835,7 @@
         <v>342</v>
       </c>
       <c r="B376" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>3</v>
@@ -5843,7 +5846,7 @@
         <v>342</v>
       </c>
       <c r="B377" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>3</v>
@@ -5854,7 +5857,7 @@
         <v>342</v>
       </c>
       <c r="B378" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C378" s="3" t="s">
         <v>3</v>
@@ -5865,7 +5868,7 @@
         <v>342</v>
       </c>
       <c r="B379" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C379" s="3" t="s">
         <v>3</v>
@@ -5876,7 +5879,7 @@
         <v>342</v>
       </c>
       <c r="B380" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C380" s="3" t="s">
         <v>3</v>
@@ -5887,7 +5890,7 @@
         <v>342</v>
       </c>
       <c r="B381" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C381" s="3" t="s">
         <v>3</v>
@@ -5898,7 +5901,7 @@
         <v>342</v>
       </c>
       <c r="B382" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C382" s="3" t="s">
         <v>3</v>
@@ -5909,7 +5912,7 @@
         <v>342</v>
       </c>
       <c r="B383" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C383" s="3" t="s">
         <v>3</v>
@@ -5920,7 +5923,7 @@
         <v>342</v>
       </c>
       <c r="B384" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C384" s="3" t="s">
         <v>3</v>
@@ -5931,7 +5934,7 @@
         <v>342</v>
       </c>
       <c r="B385" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C385" s="3" t="s">
         <v>3</v>
@@ -5942,7 +5945,7 @@
         <v>342</v>
       </c>
       <c r="B386" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C386" s="3" t="s">
         <v>3</v>
@@ -5953,7 +5956,7 @@
         <v>342</v>
       </c>
       <c r="B387" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C387" s="3" t="s">
         <v>3</v>
@@ -5964,7 +5967,7 @@
         <v>342</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C388" s="3" t="s">
         <v>3</v>
@@ -5975,7 +5978,7 @@
         <v>342</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C389" s="3" t="s">
         <v>3</v>
@@ -5986,7 +5989,7 @@
         <v>342</v>
       </c>
       <c r="B390" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C390" s="3" t="s">
         <v>3</v>
@@ -5997,7 +6000,7 @@
         <v>342</v>
       </c>
       <c r="B391" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C391" s="3" t="s">
         <v>3</v>
@@ -6008,7 +6011,7 @@
         <v>342</v>
       </c>
       <c r="B392" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C392" s="3" t="s">
         <v>3</v>
@@ -6019,7 +6022,7 @@
         <v>342</v>
       </c>
       <c r="B393" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C393" s="3" t="s">
         <v>3</v>
@@ -6030,7 +6033,7 @@
         <v>342</v>
       </c>
       <c r="B394" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C394" s="3" t="s">
         <v>3</v>
@@ -6041,7 +6044,7 @@
         <v>342</v>
       </c>
       <c r="B395" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C395" s="3" t="s">
         <v>3</v>
@@ -6052,7 +6055,7 @@
         <v>342</v>
       </c>
       <c r="B396" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C396" s="3" t="s">
         <v>3</v>
@@ -6074,7 +6077,7 @@
         <v>342</v>
       </c>
       <c r="B398" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C398" s="3" t="s">
         <v>3</v>
@@ -6085,7 +6088,7 @@
         <v>342</v>
       </c>
       <c r="B399" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C399" s="3" t="s">
         <v>3</v>
@@ -6096,7 +6099,7 @@
         <v>342</v>
       </c>
       <c r="B400" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C400" s="3" t="s">
         <v>3</v>
@@ -6107,7 +6110,7 @@
         <v>342</v>
       </c>
       <c r="B401" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C401" s="3" t="s">
         <v>3</v>
@@ -6118,7 +6121,7 @@
         <v>342</v>
       </c>
       <c r="B402" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C402" s="3" t="s">
         <v>3</v>
@@ -6129,7 +6132,7 @@
         <v>342</v>
       </c>
       <c r="B403" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C403" s="3" t="s">
         <v>3</v>
@@ -6140,7 +6143,7 @@
         <v>342</v>
       </c>
       <c r="B404" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C404" s="3" t="s">
         <v>3</v>
@@ -6151,7 +6154,7 @@
         <v>342</v>
       </c>
       <c r="B405" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C405" s="3" t="s">
         <v>3</v>
@@ -6162,37 +6165,37 @@
         <v>342</v>
       </c>
       <c r="B406" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="C406" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" ht="21">
+      <c r="A407" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B407" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="C406" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="407" spans="1:3" ht="21">
-      <c r="B407" s="6"/>
-      <c r="C407" s="3"/>
+      <c r="C407" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="408" spans="1:3" ht="21">
       <c r="B408" s="6"/>
       <c r="C408" s="3"/>
     </row>
     <row r="409" spans="1:3" ht="21">
-      <c r="A409" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="B409" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="C409" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B409" s="6"/>
+      <c r="C409" s="3"/>
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="7" t="s">
         <v>386</v>
       </c>
       <c r="B410" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C410" s="3" t="s">
         <v>3</v>
@@ -6203,7 +6206,7 @@
         <v>386</v>
       </c>
       <c r="B411" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C411" s="3" t="s">
         <v>3</v>
@@ -6214,7 +6217,7 @@
         <v>386</v>
       </c>
       <c r="B412" s="5" t="s">
-        <v>88</v>
+        <v>389</v>
       </c>
       <c r="C412" s="3" t="s">
         <v>3</v>
@@ -6225,7 +6228,7 @@
         <v>386</v>
       </c>
       <c r="B413" s="5" t="s">
-        <v>390</v>
+        <v>88</v>
       </c>
       <c r="C413" s="3" t="s">
         <v>3</v>
@@ -6236,37 +6239,37 @@
         <v>386</v>
       </c>
       <c r="B414" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C414" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" ht="21">
+      <c r="A415" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B415" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="C414" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="415" spans="1:3" ht="21">
-      <c r="B415" s="6"/>
-      <c r="C415" s="3"/>
+      <c r="C415" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="416" spans="1:3" ht="21">
       <c r="B416" s="6"/>
       <c r="C416" s="3"/>
     </row>
     <row r="417" spans="1:3" ht="21">
-      <c r="A417" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B417" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="C417" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B417" s="6"/>
+      <c r="C417" s="3"/>
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="4" t="s">
         <v>392</v>
       </c>
       <c r="B418" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C418" s="3" t="s">
         <v>3</v>
@@ -6277,7 +6280,7 @@
         <v>392</v>
       </c>
       <c r="B419" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C419" s="3" t="s">
         <v>3</v>
@@ -6288,7 +6291,7 @@
         <v>392</v>
       </c>
       <c r="B420" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C420" s="3" t="s">
         <v>3</v>
@@ -6299,7 +6302,7 @@
         <v>392</v>
       </c>
       <c r="B421" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C421" s="3" t="s">
         <v>3</v>
@@ -6310,7 +6313,7 @@
         <v>392</v>
       </c>
       <c r="B422" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C422" s="3" t="s">
         <v>3</v>
@@ -6321,7 +6324,7 @@
         <v>392</v>
       </c>
       <c r="B423" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C423" s="3" t="s">
         <v>3</v>
@@ -6332,7 +6335,7 @@
         <v>392</v>
       </c>
       <c r="B424" s="5" t="s">
-        <v>272</v>
+        <v>399</v>
       </c>
       <c r="C424" s="3" t="s">
         <v>3</v>
@@ -6343,7 +6346,7 @@
         <v>392</v>
       </c>
       <c r="B425" s="5" t="s">
-        <v>400</v>
+        <v>272</v>
       </c>
       <c r="C425" s="3" t="s">
         <v>3</v>
@@ -6354,7 +6357,7 @@
         <v>392</v>
       </c>
       <c r="B426" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C426" s="3" t="s">
         <v>3</v>
@@ -6365,7 +6368,7 @@
         <v>392</v>
       </c>
       <c r="B427" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C427" s="3" t="s">
         <v>3</v>
@@ -6376,7 +6379,7 @@
         <v>392</v>
       </c>
       <c r="B428" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C428" s="3" t="s">
         <v>3</v>
@@ -6387,7 +6390,7 @@
         <v>392</v>
       </c>
       <c r="B429" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C429" s="3" t="s">
         <v>3</v>
@@ -6398,7 +6401,7 @@
         <v>392</v>
       </c>
       <c r="B430" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C430" s="3" t="s">
         <v>3</v>
@@ -6409,7 +6412,7 @@
         <v>392</v>
       </c>
       <c r="B431" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C431" s="3" t="s">
         <v>3</v>
@@ -6420,7 +6423,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C432" s="3" t="s">
         <v>3</v>
@@ -6431,7 +6434,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C433" s="3" t="s">
         <v>3</v>
@@ -6442,7 +6445,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C434" s="3" t="s">
         <v>3</v>
@@ -6453,7 +6456,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C435" s="3" t="s">
         <v>3</v>
@@ -6464,7 +6467,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C436" s="3" t="s">
         <v>3</v>
@@ -6475,7 +6478,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C437" s="3" t="s">
         <v>3</v>
@@ -6486,7 +6489,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C438" s="3" t="s">
         <v>3</v>
@@ -6497,7 +6500,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C439" s="3" t="s">
         <v>3</v>
@@ -6508,7 +6511,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C440" s="3" t="s">
         <v>3</v>
@@ -6519,7 +6522,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C441" s="3" t="s">
         <v>3</v>
@@ -6530,7 +6533,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C442" s="3" t="s">
         <v>3</v>
@@ -6541,7 +6544,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C443" s="3" t="s">
         <v>3</v>
@@ -6552,7 +6555,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C444" s="3" t="s">
         <v>3</v>
@@ -6563,7 +6566,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C445" s="3" t="s">
         <v>3</v>
@@ -6574,7 +6577,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C446" s="3" t="s">
         <v>3</v>
@@ -6585,7 +6588,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C447" s="3" t="s">
         <v>3</v>
@@ -6596,7 +6599,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C448" s="3" t="s">
         <v>3</v>
@@ -6607,7 +6610,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C449" s="3" t="s">
         <v>3</v>
@@ -6618,7 +6621,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C450" s="3" t="s">
         <v>3</v>
@@ -6629,7 +6632,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C451" s="3" t="s">
         <v>3</v>
@@ -6640,7 +6643,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C452" s="3" t="s">
         <v>3</v>
@@ -6651,7 +6654,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C453" s="3" t="s">
         <v>3</v>
@@ -6662,7 +6665,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C454" s="3" t="s">
         <v>3</v>
@@ -6673,7 +6676,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C455" s="3" t="s">
         <v>3</v>
@@ -6684,7 +6687,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C456" s="3" t="s">
         <v>3</v>
@@ -6695,7 +6698,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C457" s="3" t="s">
         <v>3</v>
@@ -6706,7 +6709,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C458" s="3" t="s">
         <v>3</v>
@@ -6717,7 +6720,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C459" s="3" t="s">
         <v>3</v>
@@ -6728,7 +6731,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C460" s="3" t="s">
         <v>3</v>
@@ -6739,7 +6742,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C461" s="3" t="s">
         <v>3</v>
@@ -6750,7 +6753,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C462" s="3" t="s">
         <v>3</v>
@@ -6761,7 +6764,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C463" s="3" t="s">
         <v>3</v>
@@ -6772,7 +6775,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C464" s="3" t="s">
         <v>3</v>
@@ -6783,7 +6786,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C465" s="3" t="s">
         <v>3</v>
@@ -6794,7 +6797,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C466" s="3" t="s">
         <v>3</v>
@@ -6805,7 +6808,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C467" s="3" t="s">
         <v>3</v>
@@ -6816,7 +6819,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C468" s="3" t="s">
         <v>3</v>
@@ -6827,7 +6830,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C469" s="3" t="s">
         <v>3</v>
@@ -6838,7 +6841,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C470" s="3" t="s">
         <v>3</v>
@@ -6849,7 +6852,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C471" s="3" t="s">
         <v>3</v>
@@ -6860,7 +6863,7 @@
         <v>392</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C472" s="3" t="s">
         <v>3</v>
@@ -6871,7 +6874,7 @@
         <v>392</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C473" s="3" t="s">
         <v>3</v>
@@ -6882,7 +6885,7 @@
         <v>392</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C474" s="3" t="s">
         <v>3</v>
@@ -6893,7 +6896,7 @@
         <v>392</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C475" s="3" t="s">
         <v>3</v>
@@ -6904,38 +6907,38 @@
         <v>392</v>
       </c>
       <c r="B476" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="C476" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" ht="21">
+      <c r="A477" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B477" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="C476" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="477" spans="1:3" ht="21">
-      <c r="B477" s="6"/>
-      <c r="C477" s="3"/>
+      <c r="C477" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="478" spans="1:3" ht="21">
-      <c r="A478" s="7"/>
       <c r="B478" s="6"/>
       <c r="C478" s="3"/>
     </row>
     <row r="479" spans="1:3" ht="21">
-      <c r="A479" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B479" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="C479" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A479" s="7"/>
+      <c r="B479" s="6"/>
+      <c r="C479" s="3"/>
     </row>
     <row r="480" spans="1:3" ht="21">
       <c r="A480" s="4" t="s">
         <v>452</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C480" s="3" t="s">
         <v>3</v>
@@ -6946,7 +6949,7 @@
         <v>452</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C481" s="3" t="s">
         <v>3</v>
@@ -6957,7 +6960,7 @@
         <v>452</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C482" s="3" t="s">
         <v>3</v>
@@ -6968,7 +6971,7 @@
         <v>452</v>
       </c>
       <c r="B483" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C483" s="3" t="s">
         <v>3</v>
@@ -6979,7 +6982,7 @@
         <v>452</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C484" s="3" t="s">
         <v>3</v>
@@ -6990,7 +6993,7 @@
         <v>452</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C485" s="3" t="s">
         <v>3</v>
@@ -7001,7 +7004,7 @@
         <v>452</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C486" s="3" t="s">
         <v>3</v>
@@ -7012,7 +7015,7 @@
         <v>452</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C487" s="3" t="s">
         <v>3</v>
@@ -7023,9 +7026,20 @@
         <v>452</v>
       </c>
       <c r="B488" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="C488" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" ht="21">
+      <c r="A489" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B489" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="C488" s="3" t="s">
+      <c r="C489" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7189,293 +7203,293 @@
     <hyperlink ref="B178" r:id="rId156" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
     <hyperlink ref="B179" r:id="rId157" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
     <hyperlink ref="B180" r:id="rId158" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
-    <hyperlink ref="B184" r:id="rId159" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
-    <hyperlink ref="B185" r:id="rId160" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
-    <hyperlink ref="B186" r:id="rId161" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
-    <hyperlink ref="B187" r:id="rId162" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
-    <hyperlink ref="B188" r:id="rId163" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
-    <hyperlink ref="B189" r:id="rId164" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
-    <hyperlink ref="B190" r:id="rId165" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
-    <hyperlink ref="B191" r:id="rId166" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
-    <hyperlink ref="B192" r:id="rId167" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
-    <hyperlink ref="B193" r:id="rId168" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
-    <hyperlink ref="B194" r:id="rId169" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
-    <hyperlink ref="B195" r:id="rId170" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
-    <hyperlink ref="B196" r:id="rId171" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
-    <hyperlink ref="B197" r:id="rId172" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
-    <hyperlink ref="B198" r:id="rId173" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
-    <hyperlink ref="B199" r:id="rId174" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
-    <hyperlink ref="B200" r:id="rId175" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
-    <hyperlink ref="B201" r:id="rId176" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
-    <hyperlink ref="B202" r:id="rId177" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
-    <hyperlink ref="B203" r:id="rId178" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
-    <hyperlink ref="B204" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
-    <hyperlink ref="B205" r:id="rId180" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
-    <hyperlink ref="B206" r:id="rId181" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
-    <hyperlink ref="B207" r:id="rId182" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
-    <hyperlink ref="B208" r:id="rId183" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
-    <hyperlink ref="B209" r:id="rId184" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
-    <hyperlink ref="B210" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
-    <hyperlink ref="B211" r:id="rId186" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
-    <hyperlink ref="B212" r:id="rId187" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
-    <hyperlink ref="B213" r:id="rId188" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
-    <hyperlink ref="B214" r:id="rId189" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
-    <hyperlink ref="B215" r:id="rId190" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
-    <hyperlink ref="B216" r:id="rId191" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
-    <hyperlink ref="B217" r:id="rId192" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
-    <hyperlink ref="B218" r:id="rId193" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
-    <hyperlink ref="B221" r:id="rId194" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
-    <hyperlink ref="B222" r:id="rId195" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
-    <hyperlink ref="B223" r:id="rId196" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
-    <hyperlink ref="B224" r:id="rId197" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
-    <hyperlink ref="B225" r:id="rId198" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
-    <hyperlink ref="B226" r:id="rId199" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
-    <hyperlink ref="B227" r:id="rId200" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
-    <hyperlink ref="B228" r:id="rId201" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
-    <hyperlink ref="B229" r:id="rId202" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
-    <hyperlink ref="B230" r:id="rId203" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
-    <hyperlink ref="B231" r:id="rId204" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
-    <hyperlink ref="B232" r:id="rId205" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
-    <hyperlink ref="B233" r:id="rId206" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
-    <hyperlink ref="B234" r:id="rId207" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
-    <hyperlink ref="B235" r:id="rId208" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
-    <hyperlink ref="B236" r:id="rId209" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
-    <hyperlink ref="B237" r:id="rId210" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
-    <hyperlink ref="B238" r:id="rId211" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
-    <hyperlink ref="B239" r:id="rId212" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
-    <hyperlink ref="B240" r:id="rId213" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
-    <hyperlink ref="B241" r:id="rId214" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
-    <hyperlink ref="B242" r:id="rId215" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
-    <hyperlink ref="B245" r:id="rId216" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
-    <hyperlink ref="B246" r:id="rId217" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
-    <hyperlink ref="B247" r:id="rId218" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
-    <hyperlink ref="B248" r:id="rId219" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
-    <hyperlink ref="B249" r:id="rId220" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
-    <hyperlink ref="B250" r:id="rId221" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
-    <hyperlink ref="B251" r:id="rId222" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
-    <hyperlink ref="B252" r:id="rId223" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
-    <hyperlink ref="B253" r:id="rId224" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
-    <hyperlink ref="B254" r:id="rId225" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
-    <hyperlink ref="B255" r:id="rId226" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
-    <hyperlink ref="B256" r:id="rId227" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
-    <hyperlink ref="B257" r:id="rId228" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
-    <hyperlink ref="B258" r:id="rId229" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
-    <hyperlink ref="B259" r:id="rId230" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
-    <hyperlink ref="B260" r:id="rId231" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
-    <hyperlink ref="B261" r:id="rId232" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
-    <hyperlink ref="B262" r:id="rId233" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
-    <hyperlink ref="B263" r:id="rId234" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
-    <hyperlink ref="B264" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
-    <hyperlink ref="B265" r:id="rId236" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
-    <hyperlink ref="B266" r:id="rId237" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
-    <hyperlink ref="B267" r:id="rId238" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
-    <hyperlink ref="B268" r:id="rId239" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
-    <hyperlink ref="B269" r:id="rId240" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
-    <hyperlink ref="B270" r:id="rId241" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
-    <hyperlink ref="B271" r:id="rId242" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
-    <hyperlink ref="B272" r:id="rId243" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
-    <hyperlink ref="B273" r:id="rId244" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
-    <hyperlink ref="B274" r:id="rId245" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
-    <hyperlink ref="B275" r:id="rId246" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
-    <hyperlink ref="B276" r:id="rId247" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
-    <hyperlink ref="B277" r:id="rId248" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
-    <hyperlink ref="B278" r:id="rId249" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
-    <hyperlink ref="B279" r:id="rId250" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
-    <hyperlink ref="B282" r:id="rId251" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
-    <hyperlink ref="B283" r:id="rId252" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
-    <hyperlink ref="B284" r:id="rId253" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
-    <hyperlink ref="B285" r:id="rId254" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
-    <hyperlink ref="B286" r:id="rId255" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
-    <hyperlink ref="B287" r:id="rId256" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
-    <hyperlink ref="B288" r:id="rId257" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
-    <hyperlink ref="B289" r:id="rId258" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
-    <hyperlink ref="B290" r:id="rId259" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
-    <hyperlink ref="B291" r:id="rId260" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
-    <hyperlink ref="B292" r:id="rId261" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
-    <hyperlink ref="B293" r:id="rId262" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
-    <hyperlink ref="B294" r:id="rId263" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
-    <hyperlink ref="B295" r:id="rId264" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
-    <hyperlink ref="B296" r:id="rId265" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
-    <hyperlink ref="B297" r:id="rId266" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
-    <hyperlink ref="B298" r:id="rId267" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
-    <hyperlink ref="B299" r:id="rId268" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
-    <hyperlink ref="B300" r:id="rId269" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
-    <hyperlink ref="B303" r:id="rId270" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
-    <hyperlink ref="B304" r:id="rId271" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
-    <hyperlink ref="B305" r:id="rId272" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
-    <hyperlink ref="B306" r:id="rId273" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
-    <hyperlink ref="B307" r:id="rId274" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
-    <hyperlink ref="B308" r:id="rId275" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
-    <hyperlink ref="B309" r:id="rId276" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
-    <hyperlink ref="B310" r:id="rId277" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
-    <hyperlink ref="B311" r:id="rId278" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
-    <hyperlink ref="B312" r:id="rId279" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
-    <hyperlink ref="B313" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
-    <hyperlink ref="B314" r:id="rId281" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
-    <hyperlink ref="B315" r:id="rId282" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
-    <hyperlink ref="B316" r:id="rId283" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
-    <hyperlink ref="B317" r:id="rId284" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
-    <hyperlink ref="B318" r:id="rId285" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
-    <hyperlink ref="B319" r:id="rId286" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
-    <hyperlink ref="B320" r:id="rId287" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
-    <hyperlink ref="B321" r:id="rId288" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
-    <hyperlink ref="B322" r:id="rId289" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
-    <hyperlink ref="B323" r:id="rId290" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
-    <hyperlink ref="B324" r:id="rId291" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
-    <hyperlink ref="B325" r:id="rId292" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
-    <hyperlink ref="B326" r:id="rId293" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
-    <hyperlink ref="B327" r:id="rId294" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
-    <hyperlink ref="B328" r:id="rId295" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
-    <hyperlink ref="B329" r:id="rId296" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
-    <hyperlink ref="B330" r:id="rId297" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
-    <hyperlink ref="B331" r:id="rId298" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
-    <hyperlink ref="B332" r:id="rId299" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
-    <hyperlink ref="B333" r:id="rId300" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
-    <hyperlink ref="B334" r:id="rId301" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
-    <hyperlink ref="B335" r:id="rId302" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
-    <hyperlink ref="B336" r:id="rId303" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
-    <hyperlink ref="B337" r:id="rId304" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
-    <hyperlink ref="B338" r:id="rId305" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
-    <hyperlink ref="B339" r:id="rId306" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
-    <hyperlink ref="B340" r:id="rId307" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
-    <hyperlink ref="B343" r:id="rId308" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
-    <hyperlink ref="B344" r:id="rId309" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
-    <hyperlink ref="B345" r:id="rId310" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
-    <hyperlink ref="B346" r:id="rId311" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
-    <hyperlink ref="B347" r:id="rId312" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
-    <hyperlink ref="B348" r:id="rId313" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
-    <hyperlink ref="B349" r:id="rId314" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
-    <hyperlink ref="B350" r:id="rId315" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
-    <hyperlink ref="B351" r:id="rId316" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
-    <hyperlink ref="B352" r:id="rId317" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
-    <hyperlink ref="B353" r:id="rId318" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
-    <hyperlink ref="B354" r:id="rId319" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
-    <hyperlink ref="B355" r:id="rId320" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
-    <hyperlink ref="B356" r:id="rId321" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
-    <hyperlink ref="B357" r:id="rId322" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
-    <hyperlink ref="B358" r:id="rId323" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
-    <hyperlink ref="B359" r:id="rId324" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
-    <hyperlink ref="B360" r:id="rId325" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
-    <hyperlink ref="B364" r:id="rId326" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
-    <hyperlink ref="B365" r:id="rId327" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
-    <hyperlink ref="B366" r:id="rId328" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
-    <hyperlink ref="B367" r:id="rId329" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
-    <hyperlink ref="B368" r:id="rId330" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
-    <hyperlink ref="B369" r:id="rId331" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
-    <hyperlink ref="B370" r:id="rId332" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
-    <hyperlink ref="B371" r:id="rId333" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
-    <hyperlink ref="B372" r:id="rId334" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
-    <hyperlink ref="B373" r:id="rId335" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
-    <hyperlink ref="B374" r:id="rId336" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
-    <hyperlink ref="B375" r:id="rId337" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
-    <hyperlink ref="B376" r:id="rId338" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
-    <hyperlink ref="B377" r:id="rId339" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
-    <hyperlink ref="B378" r:id="rId340" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
-    <hyperlink ref="B379" r:id="rId341" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
-    <hyperlink ref="B380" r:id="rId342" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="B381" r:id="rId343" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="B382" r:id="rId344" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="B383" r:id="rId345" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="B384" r:id="rId346" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="B385" r:id="rId347" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="B386" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="B387" r:id="rId349" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="B388" r:id="rId350" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="B389" r:id="rId351" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="B390" r:id="rId352" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="B391" r:id="rId353" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="B392" r:id="rId354" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="B393" r:id="rId355" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="B394" r:id="rId356" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="B395" r:id="rId357" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="B396" r:id="rId358" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="B397" r:id="rId359" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="B398" r:id="rId360" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="B399" r:id="rId361" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="B400" r:id="rId362" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="B401" r:id="rId363" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="B403" r:id="rId364" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="B402" r:id="rId365" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="B404" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="B405" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="B406" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B409" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B410" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B411" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B412" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B413" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B414" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B417" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B418" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B419" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B420" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B421" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B422" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B423" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B424" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B425" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B426" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B427" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B428" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B429" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B430" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B431" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B432" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B433" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B434" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B435" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B436" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B437" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B438" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B439" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B440" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B441" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B442" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B443" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B444" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B445" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B446" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B447" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B448" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B449" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B450" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B451" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B452" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B453" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B454" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B455" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B456" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B458" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B457" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B459" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B460" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B461" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B462" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B463" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B464" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B465" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B466" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B467" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B468" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B469" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B476" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B475" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B474" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B473" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B472" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B471" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B470" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B479" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B480" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B481" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B482" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B483" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B484" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B485" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B488" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B486" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B487" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="B363" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
+    <hyperlink ref="B185" r:id="rId159" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
+    <hyperlink ref="B186" r:id="rId160" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
+    <hyperlink ref="B187" r:id="rId161" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
+    <hyperlink ref="B188" r:id="rId162" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
+    <hyperlink ref="B189" r:id="rId163" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
+    <hyperlink ref="B190" r:id="rId164" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
+    <hyperlink ref="B191" r:id="rId165" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
+    <hyperlink ref="B192" r:id="rId166" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
+    <hyperlink ref="B193" r:id="rId167" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
+    <hyperlink ref="B194" r:id="rId168" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
+    <hyperlink ref="B195" r:id="rId169" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
+    <hyperlink ref="B196" r:id="rId170" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
+    <hyperlink ref="B197" r:id="rId171" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
+    <hyperlink ref="B198" r:id="rId172" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
+    <hyperlink ref="B199" r:id="rId173" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
+    <hyperlink ref="B200" r:id="rId174" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
+    <hyperlink ref="B201" r:id="rId175" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
+    <hyperlink ref="B202" r:id="rId176" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
+    <hyperlink ref="B203" r:id="rId177" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
+    <hyperlink ref="B204" r:id="rId178" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
+    <hyperlink ref="B205" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
+    <hyperlink ref="B206" r:id="rId180" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
+    <hyperlink ref="B207" r:id="rId181" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
+    <hyperlink ref="B208" r:id="rId182" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
+    <hyperlink ref="B209" r:id="rId183" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
+    <hyperlink ref="B210" r:id="rId184" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
+    <hyperlink ref="B211" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
+    <hyperlink ref="B212" r:id="rId186" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
+    <hyperlink ref="B213" r:id="rId187" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
+    <hyperlink ref="B214" r:id="rId188" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
+    <hyperlink ref="B215" r:id="rId189" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
+    <hyperlink ref="B216" r:id="rId190" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
+    <hyperlink ref="B217" r:id="rId191" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
+    <hyperlink ref="B218" r:id="rId192" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
+    <hyperlink ref="B219" r:id="rId193" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
+    <hyperlink ref="B222" r:id="rId194" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
+    <hyperlink ref="B223" r:id="rId195" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
+    <hyperlink ref="B224" r:id="rId196" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
+    <hyperlink ref="B225" r:id="rId197" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
+    <hyperlink ref="B226" r:id="rId198" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
+    <hyperlink ref="B227" r:id="rId199" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
+    <hyperlink ref="B228" r:id="rId200" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
+    <hyperlink ref="B229" r:id="rId201" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
+    <hyperlink ref="B230" r:id="rId202" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
+    <hyperlink ref="B231" r:id="rId203" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
+    <hyperlink ref="B232" r:id="rId204" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
+    <hyperlink ref="B233" r:id="rId205" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
+    <hyperlink ref="B234" r:id="rId206" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
+    <hyperlink ref="B235" r:id="rId207" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
+    <hyperlink ref="B236" r:id="rId208" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
+    <hyperlink ref="B237" r:id="rId209" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
+    <hyperlink ref="B238" r:id="rId210" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
+    <hyperlink ref="B239" r:id="rId211" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
+    <hyperlink ref="B240" r:id="rId212" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
+    <hyperlink ref="B241" r:id="rId213" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
+    <hyperlink ref="B242" r:id="rId214" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
+    <hyperlink ref="B243" r:id="rId215" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
+    <hyperlink ref="B246" r:id="rId216" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
+    <hyperlink ref="B247" r:id="rId217" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
+    <hyperlink ref="B248" r:id="rId218" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
+    <hyperlink ref="B249" r:id="rId219" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
+    <hyperlink ref="B250" r:id="rId220" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
+    <hyperlink ref="B251" r:id="rId221" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
+    <hyperlink ref="B252" r:id="rId222" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
+    <hyperlink ref="B253" r:id="rId223" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
+    <hyperlink ref="B254" r:id="rId224" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
+    <hyperlink ref="B255" r:id="rId225" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
+    <hyperlink ref="B256" r:id="rId226" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
+    <hyperlink ref="B257" r:id="rId227" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
+    <hyperlink ref="B258" r:id="rId228" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
+    <hyperlink ref="B259" r:id="rId229" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
+    <hyperlink ref="B260" r:id="rId230" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
+    <hyperlink ref="B261" r:id="rId231" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
+    <hyperlink ref="B262" r:id="rId232" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
+    <hyperlink ref="B263" r:id="rId233" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
+    <hyperlink ref="B264" r:id="rId234" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
+    <hyperlink ref="B265" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
+    <hyperlink ref="B266" r:id="rId236" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
+    <hyperlink ref="B267" r:id="rId237" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
+    <hyperlink ref="B268" r:id="rId238" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
+    <hyperlink ref="B269" r:id="rId239" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
+    <hyperlink ref="B270" r:id="rId240" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
+    <hyperlink ref="B271" r:id="rId241" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
+    <hyperlink ref="B272" r:id="rId242" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
+    <hyperlink ref="B273" r:id="rId243" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
+    <hyperlink ref="B274" r:id="rId244" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
+    <hyperlink ref="B275" r:id="rId245" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
+    <hyperlink ref="B276" r:id="rId246" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
+    <hyperlink ref="B277" r:id="rId247" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
+    <hyperlink ref="B278" r:id="rId248" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
+    <hyperlink ref="B279" r:id="rId249" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
+    <hyperlink ref="B280" r:id="rId250" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
+    <hyperlink ref="B283" r:id="rId251" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
+    <hyperlink ref="B284" r:id="rId252" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
+    <hyperlink ref="B285" r:id="rId253" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
+    <hyperlink ref="B286" r:id="rId254" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
+    <hyperlink ref="B287" r:id="rId255" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
+    <hyperlink ref="B288" r:id="rId256" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
+    <hyperlink ref="B289" r:id="rId257" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
+    <hyperlink ref="B290" r:id="rId258" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
+    <hyperlink ref="B291" r:id="rId259" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
+    <hyperlink ref="B292" r:id="rId260" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
+    <hyperlink ref="B293" r:id="rId261" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
+    <hyperlink ref="B294" r:id="rId262" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
+    <hyperlink ref="B295" r:id="rId263" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
+    <hyperlink ref="B296" r:id="rId264" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
+    <hyperlink ref="B297" r:id="rId265" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
+    <hyperlink ref="B298" r:id="rId266" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
+    <hyperlink ref="B299" r:id="rId267" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
+    <hyperlink ref="B300" r:id="rId268" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="B301" r:id="rId269" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
+    <hyperlink ref="B304" r:id="rId270" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
+    <hyperlink ref="B305" r:id="rId271" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
+    <hyperlink ref="B306" r:id="rId272" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
+    <hyperlink ref="B307" r:id="rId273" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
+    <hyperlink ref="B308" r:id="rId274" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
+    <hyperlink ref="B309" r:id="rId275" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
+    <hyperlink ref="B310" r:id="rId276" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
+    <hyperlink ref="B311" r:id="rId277" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
+    <hyperlink ref="B312" r:id="rId278" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
+    <hyperlink ref="B313" r:id="rId279" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
+    <hyperlink ref="B314" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
+    <hyperlink ref="B315" r:id="rId281" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
+    <hyperlink ref="B316" r:id="rId282" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
+    <hyperlink ref="B317" r:id="rId283" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
+    <hyperlink ref="B318" r:id="rId284" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
+    <hyperlink ref="B319" r:id="rId285" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
+    <hyperlink ref="B320" r:id="rId286" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
+    <hyperlink ref="B321" r:id="rId287" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
+    <hyperlink ref="B322" r:id="rId288" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
+    <hyperlink ref="B323" r:id="rId289" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
+    <hyperlink ref="B324" r:id="rId290" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
+    <hyperlink ref="B325" r:id="rId291" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
+    <hyperlink ref="B326" r:id="rId292" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
+    <hyperlink ref="B327" r:id="rId293" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
+    <hyperlink ref="B328" r:id="rId294" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
+    <hyperlink ref="B329" r:id="rId295" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
+    <hyperlink ref="B330" r:id="rId296" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
+    <hyperlink ref="B331" r:id="rId297" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
+    <hyperlink ref="B332" r:id="rId298" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
+    <hyperlink ref="B333" r:id="rId299" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
+    <hyperlink ref="B334" r:id="rId300" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
+    <hyperlink ref="B335" r:id="rId301" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
+    <hyperlink ref="B336" r:id="rId302" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
+    <hyperlink ref="B337" r:id="rId303" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
+    <hyperlink ref="B338" r:id="rId304" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
+    <hyperlink ref="B339" r:id="rId305" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
+    <hyperlink ref="B340" r:id="rId306" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
+    <hyperlink ref="B341" r:id="rId307" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
+    <hyperlink ref="B344" r:id="rId308" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
+    <hyperlink ref="B345" r:id="rId309" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
+    <hyperlink ref="B346" r:id="rId310" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
+    <hyperlink ref="B347" r:id="rId311" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
+    <hyperlink ref="B348" r:id="rId312" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
+    <hyperlink ref="B349" r:id="rId313" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
+    <hyperlink ref="B350" r:id="rId314" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
+    <hyperlink ref="B351" r:id="rId315" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
+    <hyperlink ref="B352" r:id="rId316" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
+    <hyperlink ref="B353" r:id="rId317" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
+    <hyperlink ref="B354" r:id="rId318" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
+    <hyperlink ref="B355" r:id="rId319" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
+    <hyperlink ref="B356" r:id="rId320" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
+    <hyperlink ref="B357" r:id="rId321" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
+    <hyperlink ref="B358" r:id="rId322" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
+    <hyperlink ref="B359" r:id="rId323" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
+    <hyperlink ref="B360" r:id="rId324" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
+    <hyperlink ref="B361" r:id="rId325" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
+    <hyperlink ref="B365" r:id="rId326" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
+    <hyperlink ref="B366" r:id="rId327" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
+    <hyperlink ref="B367" r:id="rId328" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
+    <hyperlink ref="B368" r:id="rId329" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
+    <hyperlink ref="B369" r:id="rId330" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
+    <hyperlink ref="B370" r:id="rId331" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
+    <hyperlink ref="B371" r:id="rId332" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
+    <hyperlink ref="B372" r:id="rId333" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
+    <hyperlink ref="B373" r:id="rId334" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
+    <hyperlink ref="B374" r:id="rId335" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
+    <hyperlink ref="B375" r:id="rId336" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
+    <hyperlink ref="B376" r:id="rId337" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
+    <hyperlink ref="B377" r:id="rId338" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
+    <hyperlink ref="B378" r:id="rId339" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
+    <hyperlink ref="B379" r:id="rId340" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
+    <hyperlink ref="B380" r:id="rId341" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
+    <hyperlink ref="B381" r:id="rId342" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
+    <hyperlink ref="B382" r:id="rId343" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
+    <hyperlink ref="B383" r:id="rId344" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
+    <hyperlink ref="B384" r:id="rId345" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
+    <hyperlink ref="B385" r:id="rId346" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
+    <hyperlink ref="B386" r:id="rId347" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
+    <hyperlink ref="B387" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="B388" r:id="rId349" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="B389" r:id="rId350" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="B390" r:id="rId351" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="B391" r:id="rId352" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="B392" r:id="rId353" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="B393" r:id="rId354" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="B394" r:id="rId355" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="B395" r:id="rId356" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="B396" r:id="rId357" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="B397" r:id="rId358" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="B398" r:id="rId359" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="B399" r:id="rId360" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="B400" r:id="rId361" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="B401" r:id="rId362" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="B402" r:id="rId363" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="B404" r:id="rId364" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="B403" r:id="rId365" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="B405" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="B406" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="B407" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="B410" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B411" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B412" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B413" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B414" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B415" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B418" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B419" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B420" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B421" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B422" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B423" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B424" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B425" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B426" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B427" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B428" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B429" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B430" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B431" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B432" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B433" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B434" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B435" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B436" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B437" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B438" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B439" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B440" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B441" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B442" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B443" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B444" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B445" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B446" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B447" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B448" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B449" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B450" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B451" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B452" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B453" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B454" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B455" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B456" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B457" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B459" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B458" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B460" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B461" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B462" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B463" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B464" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B465" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B466" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B467" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B468" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B469" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B470" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B477" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B476" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B475" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B474" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B473" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B472" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B471" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B480" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B481" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B482" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B483" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B484" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B485" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B486" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B489" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B487" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B488" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B364" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved "Program for n’th node from the end of a Linked List" from 450 DSA Sheet
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A54E19-0773-4C25-8DF1-C83D88878193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E35771-B4DF-4165-8A66-C5BE44CD304F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3771,7 +3771,7 @@
         <v>168</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solved "Add two Number in the form of Linked List" from 450 DSA Sheet and Also added the code for " Remove the Nth node from the end of the linked list.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E35771-B4DF-4165-8A66-C5BE44CD304F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9D793F-2571-42B4-B16F-6DC22103661B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="476">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1446,10 +1446,13 @@
     <t>Count the number of subarrays having a given XOR from Striver</t>
   </si>
   <si>
-    <t>Find Middle of the Linked List</t>
-  </si>
-  <si>
-    <t>Merge Two Sorted Linked List</t>
+    <t>Delete a Node, when the node is given in O(1) time from Striver</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Linked List from Striver</t>
+  </si>
+  <si>
+    <t>Find Middle of the Linked List from Striver</t>
   </si>
 </sst>
 </file>
@@ -1887,10 +1890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:C489"/>
+  <dimension ref="A1:C493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3496,7 +3499,7 @@
         <v>143</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21">
@@ -3790,7 +3793,7 @@
         <v>133</v>
       </c>
       <c r="B181" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C181" s="3" t="s">
         <v>465</v>
@@ -3807,60 +3810,41 @@
         <v>465</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="21">
-      <c r="B184" s="6"/>
+    <row r="183" spans="1:3" ht="19.5">
+      <c r="A183" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B183" t="s">
+        <v>473</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="19.5">
+      <c r="A184" s="7"/>
       <c r="C184" s="3"/>
     </row>
-    <row r="185" spans="1:3" ht="21">
-      <c r="A185" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B185" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="21">
-      <c r="A186" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B186" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="21">
-      <c r="A187" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B187" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C187" s="3" t="s">
-        <v>3</v>
-      </c>
+    <row r="185" spans="1:3" ht="19.5">
+      <c r="A185" s="7"/>
+      <c r="C185" s="3"/>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="C186" s="3"/>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="C187" s="3"/>
     </row>
     <row r="188" spans="1:3" ht="21">
-      <c r="A188" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B188" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B188" s="6"/>
+      <c r="C188" s="3"/>
     </row>
     <row r="189" spans="1:3" ht="21">
       <c r="A189" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>3</v>
@@ -3871,7 +3855,7 @@
         <v>170</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>3</v>
@@ -3882,7 +3866,7 @@
         <v>170</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>3</v>
@@ -3893,7 +3877,7 @@
         <v>170</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>3</v>
@@ -3904,7 +3888,7 @@
         <v>170</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>3</v>
@@ -3915,7 +3899,7 @@
         <v>170</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>3</v>
@@ -3926,7 +3910,7 @@
         <v>170</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>3</v>
@@ -3937,7 +3921,7 @@
         <v>170</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>3</v>
@@ -3948,7 +3932,7 @@
         <v>170</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>3</v>
@@ -3959,7 +3943,7 @@
         <v>170</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>3</v>
@@ -3970,7 +3954,7 @@
         <v>170</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>3</v>
@@ -3981,7 +3965,7 @@
         <v>170</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>3</v>
@@ -3992,7 +3976,7 @@
         <v>170</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>3</v>
@@ -4003,7 +3987,7 @@
         <v>170</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C202" s="3" t="s">
         <v>3</v>
@@ -4014,7 +3998,7 @@
         <v>170</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>3</v>
@@ -4025,7 +4009,7 @@
         <v>170</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>3</v>
@@ -4036,7 +4020,7 @@
         <v>170</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>3</v>
@@ -4047,7 +4031,7 @@
         <v>170</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>3</v>
@@ -4058,7 +4042,7 @@
         <v>170</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>3</v>
@@ -4069,7 +4053,7 @@
         <v>170</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>3</v>
@@ -4080,7 +4064,7 @@
         <v>170</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>3</v>
@@ -4091,7 +4075,7 @@
         <v>170</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>3</v>
@@ -4102,7 +4086,7 @@
         <v>170</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>3</v>
@@ -4113,7 +4097,7 @@
         <v>170</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>3</v>
@@ -4124,7 +4108,7 @@
         <v>170</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>3</v>
@@ -4135,7 +4119,7 @@
         <v>170</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>3</v>
@@ -4146,7 +4130,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>3</v>
@@ -4157,7 +4141,7 @@
         <v>170</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>3</v>
@@ -4168,7 +4152,7 @@
         <v>170</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>3</v>
@@ -4179,7 +4163,7 @@
         <v>170</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>3</v>
@@ -4190,28 +4174,40 @@
         <v>170</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="21">
-      <c r="A220" s="7"/>
-      <c r="B220" s="6"/>
-      <c r="C220" s="3"/>
+      <c r="A220" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B220" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="221" spans="1:3" ht="21">
-      <c r="A221" s="7"/>
-      <c r="B221" s="6"/>
-      <c r="C221" s="3"/>
+      <c r="A221" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B221" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="222" spans="1:3" ht="21">
       <c r="A222" s="4" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>3</v>
@@ -4219,43 +4215,31 @@
     </row>
     <row r="223" spans="1:3" ht="21">
       <c r="A223" s="4" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="21">
-      <c r="A224" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B224" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C224" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A224" s="7"/>
+      <c r="B224" s="6"/>
+      <c r="C224" s="3"/>
     </row>
     <row r="225" spans="1:3" ht="21">
-      <c r="A225" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B225" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C225" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A225" s="7"/>
+      <c r="B225" s="6"/>
+      <c r="C225" s="3"/>
     </row>
     <row r="226" spans="1:3" ht="21">
       <c r="A226" s="4" t="s">
         <v>206</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>3</v>
@@ -4266,7 +4250,7 @@
         <v>206</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>3</v>
@@ -4276,8 +4260,8 @@
       <c r="A228" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B228" s="8" t="s">
-        <v>213</v>
+      <c r="B228" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="C228" s="3" t="s">
         <v>3</v>
@@ -4288,7 +4272,7 @@
         <v>206</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>3</v>
@@ -4299,7 +4283,7 @@
         <v>206</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>3</v>
@@ -4310,7 +4294,7 @@
         <v>206</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>3</v>
@@ -4320,8 +4304,8 @@
       <c r="A232" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B232" s="5" t="s">
-        <v>217</v>
+      <c r="B232" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>3</v>
@@ -4332,7 +4316,7 @@
         <v>206</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>3</v>
@@ -4343,7 +4327,7 @@
         <v>206</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>3</v>
@@ -4354,7 +4338,7 @@
         <v>206</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>3</v>
@@ -4365,7 +4349,7 @@
         <v>206</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>3</v>
@@ -4376,7 +4360,7 @@
         <v>206</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>3</v>
@@ -4387,7 +4371,7 @@
         <v>206</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>3</v>
@@ -4398,7 +4382,7 @@
         <v>206</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>3</v>
@@ -4409,7 +4393,7 @@
         <v>206</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>3</v>
@@ -4420,7 +4404,7 @@
         <v>206</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C241" s="3" t="s">
         <v>3</v>
@@ -4431,7 +4415,7 @@
         <v>206</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C242" s="3" t="s">
         <v>3</v>
@@ -4442,26 +4426,40 @@
         <v>206</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="244" spans="1:3" ht="21">
-      <c r="B244" s="6"/>
-      <c r="C244" s="3"/>
+      <c r="A244" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B244" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="245" spans="1:3" ht="21">
-      <c r="B245" s="6"/>
-      <c r="C245" s="3"/>
+      <c r="A245" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="246" spans="1:3" ht="21">
       <c r="A246" s="4" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>3</v>
@@ -4469,43 +4467,29 @@
     </row>
     <row r="247" spans="1:3" ht="21">
       <c r="A247" s="4" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="21">
-      <c r="A248" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B248" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="C248" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B248" s="6"/>
+      <c r="C248" s="3"/>
     </row>
     <row r="249" spans="1:3" ht="21">
-      <c r="A249" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B249" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="C249" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B249" s="6"/>
+      <c r="C249" s="3"/>
     </row>
     <row r="250" spans="1:3" ht="21">
       <c r="A250" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C250" s="3" t="s">
         <v>3</v>
@@ -4516,7 +4500,7 @@
         <v>229</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C251" s="3" t="s">
         <v>3</v>
@@ -4527,7 +4511,7 @@
         <v>229</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C252" s="3" t="s">
         <v>3</v>
@@ -4538,7 +4522,7 @@
         <v>229</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C253" s="3" t="s">
         <v>3</v>
@@ -4549,7 +4533,7 @@
         <v>229</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>3</v>
@@ -4560,7 +4544,7 @@
         <v>229</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>3</v>
@@ -4571,7 +4555,7 @@
         <v>229</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>3</v>
@@ -4582,7 +4566,7 @@
         <v>229</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>3</v>
@@ -4593,7 +4577,7 @@
         <v>229</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>3</v>
@@ -4604,7 +4588,7 @@
         <v>229</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>3</v>
@@ -4615,7 +4599,7 @@
         <v>229</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>3</v>
@@ -4626,7 +4610,7 @@
         <v>229</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>3</v>
@@ -4637,7 +4621,7 @@
         <v>229</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C262" s="3" t="s">
         <v>3</v>
@@ -4648,7 +4632,7 @@
         <v>229</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>3</v>
@@ -4659,7 +4643,7 @@
         <v>229</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C264" s="3" t="s">
         <v>3</v>
@@ -4670,7 +4654,7 @@
         <v>229</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>3</v>
@@ -4681,7 +4665,7 @@
         <v>229</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>3</v>
@@ -4692,7 +4676,7 @@
         <v>229</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>3</v>
@@ -4703,7 +4687,7 @@
         <v>229</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C268" s="3" t="s">
         <v>3</v>
@@ -4714,7 +4698,7 @@
         <v>229</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C269" s="3" t="s">
         <v>3</v>
@@ -4725,7 +4709,7 @@
         <v>229</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C270" s="3" t="s">
         <v>3</v>
@@ -4736,7 +4720,7 @@
         <v>229</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C271" s="3" t="s">
         <v>3</v>
@@ -4747,7 +4731,7 @@
         <v>229</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>3</v>
@@ -4758,7 +4742,7 @@
         <v>229</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>3</v>
@@ -4769,7 +4753,7 @@
         <v>229</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C274" s="3" t="s">
         <v>3</v>
@@ -4780,7 +4764,7 @@
         <v>229</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>3</v>
@@ -4791,7 +4775,7 @@
         <v>229</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C276" s="3" t="s">
         <v>3</v>
@@ -4802,7 +4786,7 @@
         <v>229</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C277" s="3" t="s">
         <v>3</v>
@@ -4813,7 +4797,7 @@
         <v>229</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C278" s="3" t="s">
         <v>3</v>
@@ -4824,7 +4808,7 @@
         <v>229</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="C279" s="3" t="s">
         <v>3</v>
@@ -4835,26 +4819,40 @@
         <v>229</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C280" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="21">
-      <c r="B281" s="6"/>
-      <c r="C281" s="3"/>
+      <c r="A281" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B281" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C281" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="282" spans="1:3" ht="21">
-      <c r="B282" s="6"/>
-      <c r="C282" s="3"/>
+      <c r="A282" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C282" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="283" spans="1:3" ht="21">
       <c r="A283" s="4" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>265</v>
+        <v>86</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>3</v>
@@ -4862,43 +4860,29 @@
     </row>
     <row r="284" spans="1:3" ht="21">
       <c r="A284" s="4" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="285" spans="1:3" ht="21">
-      <c r="A285" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B285" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C285" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B285" s="6"/>
+      <c r="C285" s="3"/>
     </row>
     <row r="286" spans="1:3" ht="21">
-      <c r="A286" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B286" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="C286" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B286" s="6"/>
+      <c r="C286" s="3"/>
     </row>
     <row r="287" spans="1:3" ht="21">
       <c r="A287" s="4" t="s">
         <v>264</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C287" s="3" t="s">
         <v>3</v>
@@ -4909,7 +4893,7 @@
         <v>264</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>3</v>
@@ -4920,7 +4904,7 @@
         <v>264</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C289" s="3" t="s">
         <v>3</v>
@@ -4931,7 +4915,7 @@
         <v>264</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C290" s="3" t="s">
         <v>3</v>
@@ -4942,7 +4926,7 @@
         <v>264</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>3</v>
@@ -4953,7 +4937,7 @@
         <v>264</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>3</v>
@@ -4964,7 +4948,7 @@
         <v>264</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C293" s="3" t="s">
         <v>3</v>
@@ -4975,7 +4959,7 @@
         <v>264</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C294" s="3" t="s">
         <v>3</v>
@@ -4986,7 +4970,7 @@
         <v>264</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C295" s="3" t="s">
         <v>3</v>
@@ -4997,7 +4981,7 @@
         <v>264</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C296" s="3" t="s">
         <v>3</v>
@@ -5008,7 +4992,7 @@
         <v>264</v>
       </c>
       <c r="B297" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C297" s="3" t="s">
         <v>3</v>
@@ -5019,7 +5003,7 @@
         <v>264</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C298" s="3" t="s">
         <v>3</v>
@@ -5030,7 +5014,7 @@
         <v>264</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C299" s="3" t="s">
         <v>3</v>
@@ -5041,7 +5025,7 @@
         <v>264</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C300" s="3" t="s">
         <v>3</v>
@@ -5052,26 +5036,40 @@
         <v>264</v>
       </c>
       <c r="B301" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C301" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="21">
-      <c r="B302" s="6"/>
-      <c r="C302" s="3"/>
+      <c r="A302" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C302" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="303" spans="1:3" ht="21">
-      <c r="B303" s="6"/>
-      <c r="C303" s="3"/>
+      <c r="A303" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B303" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C303" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="304" spans="1:3" ht="21">
       <c r="A304" s="4" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C304" s="3" t="s">
         <v>3</v>
@@ -5079,43 +5077,29 @@
     </row>
     <row r="305" spans="1:3" ht="21">
       <c r="A305" s="4" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C305" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="306" spans="1:3" ht="21">
-      <c r="A306" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B306" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="C306" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B306" s="6"/>
+      <c r="C306" s="3"/>
     </row>
     <row r="307" spans="1:3" ht="21">
-      <c r="A307" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B307" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C307" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B307" s="6"/>
+      <c r="C307" s="3"/>
     </row>
     <row r="308" spans="1:3" ht="21">
       <c r="A308" s="4" t="s">
         <v>284</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C308" s="3" t="s">
         <v>3</v>
@@ -5126,7 +5110,7 @@
         <v>284</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C309" s="3" t="s">
         <v>3</v>
@@ -5137,7 +5121,7 @@
         <v>284</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C310" s="3" t="s">
         <v>3</v>
@@ -5148,7 +5132,7 @@
         <v>284</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C311" s="3" t="s">
         <v>3</v>
@@ -5159,7 +5143,7 @@
         <v>284</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>3</v>
@@ -5170,7 +5154,7 @@
         <v>284</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C313" s="3" t="s">
         <v>3</v>
@@ -5181,7 +5165,7 @@
         <v>284</v>
       </c>
       <c r="B314" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>3</v>
@@ -5192,7 +5176,7 @@
         <v>284</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>3</v>
@@ -5203,7 +5187,7 @@
         <v>284</v>
       </c>
       <c r="B316" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C316" s="3" t="s">
         <v>3</v>
@@ -5213,8 +5197,8 @@
       <c r="A317" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B317" s="8" t="s">
-        <v>298</v>
+      <c r="B317" s="5" t="s">
+        <v>294</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>3</v>
@@ -5225,7 +5209,7 @@
         <v>284</v>
       </c>
       <c r="B318" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>3</v>
@@ -5236,7 +5220,7 @@
         <v>284</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>3</v>
@@ -5247,7 +5231,7 @@
         <v>284</v>
       </c>
       <c r="B320" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C320" s="3" t="s">
         <v>3</v>
@@ -5257,8 +5241,8 @@
       <c r="A321" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B321" s="5" t="s">
-        <v>302</v>
+      <c r="B321" s="8" t="s">
+        <v>298</v>
       </c>
       <c r="C321" s="3" t="s">
         <v>3</v>
@@ -5269,7 +5253,7 @@
         <v>284</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C322" s="3" t="s">
         <v>3</v>
@@ -5280,7 +5264,7 @@
         <v>284</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C323" s="3" t="s">
         <v>3</v>
@@ -5291,7 +5275,7 @@
         <v>284</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C324" s="3" t="s">
         <v>3</v>
@@ -5302,7 +5286,7 @@
         <v>284</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C325" s="3" t="s">
         <v>3</v>
@@ -5313,7 +5297,7 @@
         <v>284</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>3</v>
@@ -5324,7 +5308,7 @@
         <v>284</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C327" s="3" t="s">
         <v>3</v>
@@ -5335,7 +5319,7 @@
         <v>284</v>
       </c>
       <c r="B328" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>3</v>
@@ -5346,7 +5330,7 @@
         <v>284</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C329" s="3" t="s">
         <v>3</v>
@@ -5357,7 +5341,7 @@
         <v>284</v>
       </c>
       <c r="B330" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C330" s="3" t="s">
         <v>3</v>
@@ -5368,7 +5352,7 @@
         <v>284</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C331" s="3" t="s">
         <v>3</v>
@@ -5379,7 +5363,7 @@
         <v>284</v>
       </c>
       <c r="B332" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>3</v>
@@ -5390,7 +5374,7 @@
         <v>284</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C333" s="3" t="s">
         <v>3</v>
@@ -5401,7 +5385,7 @@
         <v>284</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C334" s="3" t="s">
         <v>3</v>
@@ -5412,7 +5396,7 @@
         <v>284</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C335" s="3" t="s">
         <v>3</v>
@@ -5423,7 +5407,7 @@
         <v>284</v>
       </c>
       <c r="B336" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C336" s="3" t="s">
         <v>3</v>
@@ -5434,7 +5418,7 @@
         <v>284</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C337" s="3" t="s">
         <v>3</v>
@@ -5445,7 +5429,7 @@
         <v>284</v>
       </c>
       <c r="B338" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C338" s="3" t="s">
         <v>3</v>
@@ -5456,7 +5440,7 @@
         <v>284</v>
       </c>
       <c r="B339" s="5" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C339" s="3" t="s">
         <v>3</v>
@@ -5467,7 +5451,7 @@
         <v>284</v>
       </c>
       <c r="B340" s="5" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C340" s="3" t="s">
         <v>3</v>
@@ -5478,70 +5462,70 @@
         <v>284</v>
       </c>
       <c r="B341" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C341" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" ht="21">
+      <c r="A342" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B342" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C342" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" ht="21">
+      <c r="A343" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B343" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C343" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" ht="21">
+      <c r="A344" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B344" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C344" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" ht="21">
+      <c r="A345" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B345" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="C341" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="342" spans="1:3" ht="21">
-      <c r="B342" s="6"/>
-      <c r="C342" s="3"/>
-    </row>
-    <row r="343" spans="1:3" ht="21">
-      <c r="B343" s="6"/>
-      <c r="C343" s="3"/>
-    </row>
-    <row r="344" spans="1:3" ht="21">
-      <c r="A344" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B344" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="C344" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3" ht="21">
-      <c r="A345" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B345" s="5" t="s">
-        <v>325</v>
-      </c>
       <c r="C345" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="21">
-      <c r="A346" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B346" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="C346" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B346" s="6"/>
+      <c r="C346" s="3"/>
     </row>
     <row r="347" spans="1:3" ht="21">
-      <c r="A347" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B347" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="C347" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B347" s="6"/>
+      <c r="C347" s="3"/>
     </row>
     <row r="348" spans="1:3" ht="21">
       <c r="A348" s="7" t="s">
         <v>323</v>
       </c>
       <c r="B348" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C348" s="3" t="s">
         <v>3</v>
@@ -5552,7 +5536,7 @@
         <v>323</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>3</v>
@@ -5563,7 +5547,7 @@
         <v>323</v>
       </c>
       <c r="B350" s="5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C350" s="3" t="s">
         <v>3</v>
@@ -5574,7 +5558,7 @@
         <v>323</v>
       </c>
       <c r="B351" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C351" s="3" t="s">
         <v>3</v>
@@ -5584,8 +5568,8 @@
       <c r="A352" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B352" s="8" t="s">
-        <v>332</v>
+      <c r="B352" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="C352" s="3" t="s">
         <v>3</v>
@@ -5596,7 +5580,7 @@
         <v>323</v>
       </c>
       <c r="B353" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C353" s="3" t="s">
         <v>3</v>
@@ -5607,7 +5591,7 @@
         <v>323</v>
       </c>
       <c r="B354" s="5" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C354" s="3" t="s">
         <v>3</v>
@@ -5618,7 +5602,7 @@
         <v>323</v>
       </c>
       <c r="B355" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C355" s="3" t="s">
         <v>3</v>
@@ -5628,8 +5612,8 @@
       <c r="A356" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B356" s="5" t="s">
-        <v>336</v>
+      <c r="B356" s="8" t="s">
+        <v>332</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>3</v>
@@ -5640,7 +5624,7 @@
         <v>323</v>
       </c>
       <c r="B357" s="5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C357" s="3" t="s">
         <v>3</v>
@@ -5651,7 +5635,7 @@
         <v>323</v>
       </c>
       <c r="B358" s="5" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C358" s="3" t="s">
         <v>3</v>
@@ -5662,7 +5646,7 @@
         <v>323</v>
       </c>
       <c r="B359" s="5" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C359" s="3" t="s">
         <v>3</v>
@@ -5673,7 +5657,7 @@
         <v>323</v>
       </c>
       <c r="B360" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C360" s="3" t="s">
         <v>3</v>
@@ -5684,26 +5668,40 @@
         <v>323</v>
       </c>
       <c r="B361" s="5" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C361" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="362" spans="1:3" ht="21">
-      <c r="B362" s="6"/>
-      <c r="C362" s="3"/>
+      <c r="A362" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B362" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C362" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="363" spans="1:3" ht="21">
-      <c r="B363" s="6"/>
-      <c r="C363" s="3"/>
+      <c r="A363" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B363" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="C363" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="7" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="B364" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C364" s="3" t="s">
         <v>3</v>
@@ -5711,43 +5709,29 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="7" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="B365" s="5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C365" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="366" spans="1:3" ht="21">
-      <c r="A366" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B366" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="C366" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B366" s="6"/>
+      <c r="C366" s="3"/>
     </row>
     <row r="367" spans="1:3" ht="21">
-      <c r="A367" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B367" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="C367" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B367" s="6"/>
+      <c r="C367" s="3"/>
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="7" t="s">
         <v>342</v>
       </c>
       <c r="B368" s="5" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C368" s="3" t="s">
         <v>3</v>
@@ -5758,7 +5742,7 @@
         <v>342</v>
       </c>
       <c r="B369" s="5" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C369" s="3" t="s">
         <v>3</v>
@@ -5769,7 +5753,7 @@
         <v>342</v>
       </c>
       <c r="B370" s="5" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C370" s="3" t="s">
         <v>3</v>
@@ -5780,7 +5764,7 @@
         <v>342</v>
       </c>
       <c r="B371" s="5" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C371" s="3" t="s">
         <v>3</v>
@@ -5791,7 +5775,7 @@
         <v>342</v>
       </c>
       <c r="B372" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C372" s="3" t="s">
         <v>3</v>
@@ -5802,7 +5786,7 @@
         <v>342</v>
       </c>
       <c r="B373" s="5" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>3</v>
@@ -5813,7 +5797,7 @@
         <v>342</v>
       </c>
       <c r="B374" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>3</v>
@@ -5824,7 +5808,7 @@
         <v>342</v>
       </c>
       <c r="B375" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>3</v>
@@ -5835,7 +5819,7 @@
         <v>342</v>
       </c>
       <c r="B376" s="5" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>3</v>
@@ -5846,7 +5830,7 @@
         <v>342</v>
       </c>
       <c r="B377" s="5" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>3</v>
@@ -5857,7 +5841,7 @@
         <v>342</v>
       </c>
       <c r="B378" s="5" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C378" s="3" t="s">
         <v>3</v>
@@ -5868,7 +5852,7 @@
         <v>342</v>
       </c>
       <c r="B379" s="5" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C379" s="3" t="s">
         <v>3</v>
@@ -5879,7 +5863,7 @@
         <v>342</v>
       </c>
       <c r="B380" s="5" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C380" s="3" t="s">
         <v>3</v>
@@ -5890,7 +5874,7 @@
         <v>342</v>
       </c>
       <c r="B381" s="5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C381" s="3" t="s">
         <v>3</v>
@@ -5901,7 +5885,7 @@
         <v>342</v>
       </c>
       <c r="B382" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C382" s="3" t="s">
         <v>3</v>
@@ -5912,7 +5896,7 @@
         <v>342</v>
       </c>
       <c r="B383" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C383" s="3" t="s">
         <v>3</v>
@@ -5923,7 +5907,7 @@
         <v>342</v>
       </c>
       <c r="B384" s="5" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C384" s="3" t="s">
         <v>3</v>
@@ -5934,7 +5918,7 @@
         <v>342</v>
       </c>
       <c r="B385" s="5" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C385" s="3" t="s">
         <v>3</v>
@@ -5945,7 +5929,7 @@
         <v>342</v>
       </c>
       <c r="B386" s="5" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C386" s="3" t="s">
         <v>3</v>
@@ -5956,7 +5940,7 @@
         <v>342</v>
       </c>
       <c r="B387" s="5" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C387" s="3" t="s">
         <v>3</v>
@@ -5967,7 +5951,7 @@
         <v>342</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C388" s="3" t="s">
         <v>3</v>
@@ -5978,7 +5962,7 @@
         <v>342</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C389" s="3" t="s">
         <v>3</v>
@@ -5989,7 +5973,7 @@
         <v>342</v>
       </c>
       <c r="B390" s="5" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C390" s="3" t="s">
         <v>3</v>
@@ -6000,7 +5984,7 @@
         <v>342</v>
       </c>
       <c r="B391" s="5" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C391" s="3" t="s">
         <v>3</v>
@@ -6011,7 +5995,7 @@
         <v>342</v>
       </c>
       <c r="B392" s="5" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C392" s="3" t="s">
         <v>3</v>
@@ -6022,7 +6006,7 @@
         <v>342</v>
       </c>
       <c r="B393" s="5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C393" s="3" t="s">
         <v>3</v>
@@ -6033,7 +6017,7 @@
         <v>342</v>
       </c>
       <c r="B394" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C394" s="3" t="s">
         <v>3</v>
@@ -6044,7 +6028,7 @@
         <v>342</v>
       </c>
       <c r="B395" s="5" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C395" s="3" t="s">
         <v>3</v>
@@ -6055,7 +6039,7 @@
         <v>342</v>
       </c>
       <c r="B396" s="5" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C396" s="3" t="s">
         <v>3</v>
@@ -6066,7 +6050,7 @@
         <v>342</v>
       </c>
       <c r="B397" s="5" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C397" s="3" t="s">
         <v>3</v>
@@ -6077,7 +6061,7 @@
         <v>342</v>
       </c>
       <c r="B398" s="5" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C398" s="3" t="s">
         <v>3</v>
@@ -6088,7 +6072,7 @@
         <v>342</v>
       </c>
       <c r="B399" s="5" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C399" s="3" t="s">
         <v>3</v>
@@ -6099,7 +6083,7 @@
         <v>342</v>
       </c>
       <c r="B400" s="5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C400" s="3" t="s">
         <v>3</v>
@@ -6110,7 +6094,7 @@
         <v>342</v>
       </c>
       <c r="B401" s="5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C401" s="3" t="s">
         <v>3</v>
@@ -6121,7 +6105,7 @@
         <v>342</v>
       </c>
       <c r="B402" s="5" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C402" s="3" t="s">
         <v>3</v>
@@ -6132,7 +6116,7 @@
         <v>342</v>
       </c>
       <c r="B403" s="5" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C403" s="3" t="s">
         <v>3</v>
@@ -6143,7 +6127,7 @@
         <v>342</v>
       </c>
       <c r="B404" s="5" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C404" s="3" t="s">
         <v>3</v>
@@ -6154,7 +6138,7 @@
         <v>342</v>
       </c>
       <c r="B405" s="5" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C405" s="3" t="s">
         <v>3</v>
@@ -6165,7 +6149,7 @@
         <v>342</v>
       </c>
       <c r="B406" s="5" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C406" s="3" t="s">
         <v>3</v>
@@ -6176,26 +6160,40 @@
         <v>342</v>
       </c>
       <c r="B407" s="5" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C407" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="408" spans="1:3" ht="21">
-      <c r="B408" s="6"/>
-      <c r="C408" s="3"/>
+      <c r="A408" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B408" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C408" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="409" spans="1:3" ht="21">
-      <c r="B409" s="6"/>
-      <c r="C409" s="3"/>
+      <c r="A409" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B409" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C409" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="7" t="s">
-        <v>386</v>
+        <v>342</v>
       </c>
       <c r="B410" s="5" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C410" s="3" t="s">
         <v>3</v>
@@ -6203,43 +6201,29 @@
     </row>
     <row r="411" spans="1:3" ht="21">
       <c r="A411" s="7" t="s">
-        <v>386</v>
+        <v>342</v>
       </c>
       <c r="B411" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C411" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="21">
-      <c r="A412" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="B412" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="C412" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B412" s="6"/>
+      <c r="C412" s="3"/>
     </row>
     <row r="413" spans="1:3" ht="21">
-      <c r="A413" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="B413" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C413" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B413" s="6"/>
+      <c r="C413" s="3"/>
     </row>
     <row r="414" spans="1:3" ht="21">
       <c r="A414" s="7" t="s">
         <v>386</v>
       </c>
       <c r="B414" s="5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C414" s="3" t="s">
         <v>3</v>
@@ -6250,70 +6234,70 @@
         <v>386</v>
       </c>
       <c r="B415" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="C415" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" ht="21">
+      <c r="A416" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B416" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="C416" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" ht="21">
+      <c r="A417" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B417" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C417" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" ht="21">
+      <c r="A418" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B418" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C418" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" ht="21">
+      <c r="A419" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B419" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="C415" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="416" spans="1:3" ht="21">
-      <c r="B416" s="6"/>
-      <c r="C416" s="3"/>
-    </row>
-    <row r="417" spans="1:3" ht="21">
-      <c r="B417" s="6"/>
-      <c r="C417" s="3"/>
-    </row>
-    <row r="418" spans="1:3" ht="21">
-      <c r="A418" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B418" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="C418" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="419" spans="1:3" ht="21">
-      <c r="A419" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B419" s="5" t="s">
-        <v>394</v>
-      </c>
       <c r="C419" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="21">
-      <c r="A420" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B420" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="C420" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B420" s="6"/>
+      <c r="C420" s="3"/>
     </row>
     <row r="421" spans="1:3" ht="21">
-      <c r="A421" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B421" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="C421" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B421" s="6"/>
+      <c r="C421" s="3"/>
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="4" t="s">
         <v>392</v>
       </c>
       <c r="B422" s="5" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C422" s="3" t="s">
         <v>3</v>
@@ -6324,7 +6308,7 @@
         <v>392</v>
       </c>
       <c r="B423" s="5" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C423" s="3" t="s">
         <v>3</v>
@@ -6335,7 +6319,7 @@
         <v>392</v>
       </c>
       <c r="B424" s="5" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C424" s="3" t="s">
         <v>3</v>
@@ -6346,7 +6330,7 @@
         <v>392</v>
       </c>
       <c r="B425" s="5" t="s">
-        <v>272</v>
+        <v>396</v>
       </c>
       <c r="C425" s="3" t="s">
         <v>3</v>
@@ -6357,7 +6341,7 @@
         <v>392</v>
       </c>
       <c r="B426" s="5" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C426" s="3" t="s">
         <v>3</v>
@@ -6368,7 +6352,7 @@
         <v>392</v>
       </c>
       <c r="B427" s="5" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C427" s="3" t="s">
         <v>3</v>
@@ -6379,7 +6363,7 @@
         <v>392</v>
       </c>
       <c r="B428" s="5" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C428" s="3" t="s">
         <v>3</v>
@@ -6390,7 +6374,7 @@
         <v>392</v>
       </c>
       <c r="B429" s="5" t="s">
-        <v>403</v>
+        <v>272</v>
       </c>
       <c r="C429" s="3" t="s">
         <v>3</v>
@@ -6401,7 +6385,7 @@
         <v>392</v>
       </c>
       <c r="B430" s="5" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C430" s="3" t="s">
         <v>3</v>
@@ -6412,7 +6396,7 @@
         <v>392</v>
       </c>
       <c r="B431" s="5" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C431" s="3" t="s">
         <v>3</v>
@@ -6423,7 +6407,7 @@
         <v>392</v>
       </c>
       <c r="B432" s="5" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C432" s="3" t="s">
         <v>3</v>
@@ -6434,7 +6418,7 @@
         <v>392</v>
       </c>
       <c r="B433" s="5" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C433" s="3" t="s">
         <v>3</v>
@@ -6445,7 +6429,7 @@
         <v>392</v>
       </c>
       <c r="B434" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C434" s="3" t="s">
         <v>3</v>
@@ -6456,7 +6440,7 @@
         <v>392</v>
       </c>
       <c r="B435" s="5" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C435" s="3" t="s">
         <v>3</v>
@@ -6467,7 +6451,7 @@
         <v>392</v>
       </c>
       <c r="B436" s="5" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C436" s="3" t="s">
         <v>3</v>
@@ -6478,7 +6462,7 @@
         <v>392</v>
       </c>
       <c r="B437" s="5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C437" s="3" t="s">
         <v>3</v>
@@ -6489,7 +6473,7 @@
         <v>392</v>
       </c>
       <c r="B438" s="5" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C438" s="3" t="s">
         <v>3</v>
@@ -6500,7 +6484,7 @@
         <v>392</v>
       </c>
       <c r="B439" s="5" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C439" s="3" t="s">
         <v>3</v>
@@ -6511,7 +6495,7 @@
         <v>392</v>
       </c>
       <c r="B440" s="5" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C440" s="3" t="s">
         <v>3</v>
@@ -6522,7 +6506,7 @@
         <v>392</v>
       </c>
       <c r="B441" s="5" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C441" s="3" t="s">
         <v>3</v>
@@ -6533,7 +6517,7 @@
         <v>392</v>
       </c>
       <c r="B442" s="5" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C442" s="3" t="s">
         <v>3</v>
@@ -6544,7 +6528,7 @@
         <v>392</v>
       </c>
       <c r="B443" s="5" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C443" s="3" t="s">
         <v>3</v>
@@ -6555,7 +6539,7 @@
         <v>392</v>
       </c>
       <c r="B444" s="5" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C444" s="3" t="s">
         <v>3</v>
@@ -6566,7 +6550,7 @@
         <v>392</v>
       </c>
       <c r="B445" s="5" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C445" s="3" t="s">
         <v>3</v>
@@ -6577,7 +6561,7 @@
         <v>392</v>
       </c>
       <c r="B446" s="5" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C446" s="3" t="s">
         <v>3</v>
@@ -6588,7 +6572,7 @@
         <v>392</v>
       </c>
       <c r="B447" s="5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C447" s="3" t="s">
         <v>3</v>
@@ -6599,7 +6583,7 @@
         <v>392</v>
       </c>
       <c r="B448" s="5" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C448" s="3" t="s">
         <v>3</v>
@@ -6610,7 +6594,7 @@
         <v>392</v>
       </c>
       <c r="B449" s="5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C449" s="3" t="s">
         <v>3</v>
@@ -6621,7 +6605,7 @@
         <v>392</v>
       </c>
       <c r="B450" s="5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C450" s="3" t="s">
         <v>3</v>
@@ -6632,7 +6616,7 @@
         <v>392</v>
       </c>
       <c r="B451" s="5" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C451" s="3" t="s">
         <v>3</v>
@@ -6643,7 +6627,7 @@
         <v>392</v>
       </c>
       <c r="B452" s="5" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C452" s="3" t="s">
         <v>3</v>
@@ -6654,7 +6638,7 @@
         <v>392</v>
       </c>
       <c r="B453" s="5" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C453" s="3" t="s">
         <v>3</v>
@@ -6665,7 +6649,7 @@
         <v>392</v>
       </c>
       <c r="B454" s="5" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C454" s="3" t="s">
         <v>3</v>
@@ -6676,7 +6660,7 @@
         <v>392</v>
       </c>
       <c r="B455" s="5" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C455" s="3" t="s">
         <v>3</v>
@@ -6687,7 +6671,7 @@
         <v>392</v>
       </c>
       <c r="B456" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C456" s="3" t="s">
         <v>3</v>
@@ -6698,7 +6682,7 @@
         <v>392</v>
       </c>
       <c r="B457" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C457" s="3" t="s">
         <v>3</v>
@@ -6709,7 +6693,7 @@
         <v>392</v>
       </c>
       <c r="B458" s="5" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C458" s="3" t="s">
         <v>3</v>
@@ -6720,7 +6704,7 @@
         <v>392</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C459" s="3" t="s">
         <v>3</v>
@@ -6731,7 +6715,7 @@
         <v>392</v>
       </c>
       <c r="B460" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C460" s="3" t="s">
         <v>3</v>
@@ -6742,7 +6726,7 @@
         <v>392</v>
       </c>
       <c r="B461" s="5" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C461" s="3" t="s">
         <v>3</v>
@@ -6753,7 +6737,7 @@
         <v>392</v>
       </c>
       <c r="B462" s="5" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C462" s="3" t="s">
         <v>3</v>
@@ -6764,7 +6748,7 @@
         <v>392</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C463" s="3" t="s">
         <v>3</v>
@@ -6775,7 +6759,7 @@
         <v>392</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C464" s="3" t="s">
         <v>3</v>
@@ -6786,7 +6770,7 @@
         <v>392</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C465" s="3" t="s">
         <v>3</v>
@@ -6797,7 +6781,7 @@
         <v>392</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C466" s="3" t="s">
         <v>3</v>
@@ -6808,7 +6792,7 @@
         <v>392</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C467" s="3" t="s">
         <v>3</v>
@@ -6819,7 +6803,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C468" s="3" t="s">
         <v>3</v>
@@ -6830,7 +6814,7 @@
         <v>392</v>
       </c>
       <c r="B469" s="5" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C469" s="3" t="s">
         <v>3</v>
@@ -6841,7 +6825,7 @@
         <v>392</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C470" s="3" t="s">
         <v>3</v>
@@ -6852,7 +6836,7 @@
         <v>392</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C471" s="3" t="s">
         <v>3</v>
@@ -6863,7 +6847,7 @@
         <v>392</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C472" s="3" t="s">
         <v>3</v>
@@ -6874,7 +6858,7 @@
         <v>392</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C473" s="3" t="s">
         <v>3</v>
@@ -6885,7 +6869,7 @@
         <v>392</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C474" s="3" t="s">
         <v>3</v>
@@ -6896,7 +6880,7 @@
         <v>392</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C475" s="3" t="s">
         <v>3</v>
@@ -6907,7 +6891,7 @@
         <v>392</v>
       </c>
       <c r="B476" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C476" s="3" t="s">
         <v>3</v>
@@ -6918,27 +6902,40 @@
         <v>392</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C477" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="478" spans="1:3" ht="21">
-      <c r="B478" s="6"/>
-      <c r="C478" s="3"/>
+      <c r="A478" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B478" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C478" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="479" spans="1:3" ht="21">
-      <c r="A479" s="7"/>
-      <c r="B479" s="6"/>
-      <c r="C479" s="3"/>
+      <c r="A479" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B479" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="C479" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="480" spans="1:3" ht="21">
       <c r="A480" s="4" t="s">
-        <v>452</v>
+        <v>392</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C480" s="3" t="s">
         <v>3</v>
@@ -6946,43 +6943,30 @@
     </row>
     <row r="481" spans="1:3" ht="21">
       <c r="A481" s="4" t="s">
-        <v>452</v>
+        <v>392</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C481" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="482" spans="1:3" ht="21">
-      <c r="A482" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B482" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="C482" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B482" s="6"/>
+      <c r="C482" s="3"/>
     </row>
     <row r="483" spans="1:3" ht="21">
-      <c r="A483" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B483" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="C483" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A483" s="7"/>
+      <c r="B483" s="6"/>
+      <c r="C483" s="3"/>
     </row>
     <row r="484" spans="1:3" ht="21">
       <c r="A484" s="4" t="s">
         <v>452</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C484" s="3" t="s">
         <v>3</v>
@@ -6993,7 +6977,7 @@
         <v>452</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C485" s="3" t="s">
         <v>3</v>
@@ -7004,7 +6988,7 @@
         <v>452</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C486" s="3" t="s">
         <v>3</v>
@@ -7015,7 +6999,7 @@
         <v>452</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C487" s="3" t="s">
         <v>3</v>
@@ -7026,7 +7010,7 @@
         <v>452</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C488" s="3" t="s">
         <v>3</v>
@@ -7037,9 +7021,53 @@
         <v>452</v>
       </c>
       <c r="B489" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C489" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" ht="21">
+      <c r="A490" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B490" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="C490" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" ht="21">
+      <c r="A491" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B491" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C491" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" ht="21">
+      <c r="A492" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B492" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="C492" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" ht="21">
+      <c r="A493" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B493" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="C489" s="3" t="s">
+      <c r="C493" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7203,293 +7231,293 @@
     <hyperlink ref="B178" r:id="rId156" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
     <hyperlink ref="B179" r:id="rId157" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
     <hyperlink ref="B180" r:id="rId158" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
-    <hyperlink ref="B185" r:id="rId159" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
-    <hyperlink ref="B186" r:id="rId160" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
-    <hyperlink ref="B187" r:id="rId161" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
-    <hyperlink ref="B188" r:id="rId162" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
-    <hyperlink ref="B189" r:id="rId163" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
-    <hyperlink ref="B190" r:id="rId164" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
-    <hyperlink ref="B191" r:id="rId165" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
-    <hyperlink ref="B192" r:id="rId166" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
-    <hyperlink ref="B193" r:id="rId167" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
-    <hyperlink ref="B194" r:id="rId168" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
-    <hyperlink ref="B195" r:id="rId169" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
-    <hyperlink ref="B196" r:id="rId170" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
-    <hyperlink ref="B197" r:id="rId171" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
-    <hyperlink ref="B198" r:id="rId172" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
-    <hyperlink ref="B199" r:id="rId173" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
-    <hyperlink ref="B200" r:id="rId174" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
-    <hyperlink ref="B201" r:id="rId175" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
-    <hyperlink ref="B202" r:id="rId176" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
-    <hyperlink ref="B203" r:id="rId177" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
-    <hyperlink ref="B204" r:id="rId178" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
-    <hyperlink ref="B205" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
-    <hyperlink ref="B206" r:id="rId180" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
-    <hyperlink ref="B207" r:id="rId181" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
-    <hyperlink ref="B208" r:id="rId182" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
-    <hyperlink ref="B209" r:id="rId183" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
-    <hyperlink ref="B210" r:id="rId184" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
-    <hyperlink ref="B211" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
-    <hyperlink ref="B212" r:id="rId186" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
-    <hyperlink ref="B213" r:id="rId187" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
-    <hyperlink ref="B214" r:id="rId188" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
-    <hyperlink ref="B215" r:id="rId189" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
-    <hyperlink ref="B216" r:id="rId190" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
-    <hyperlink ref="B217" r:id="rId191" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
-    <hyperlink ref="B218" r:id="rId192" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
-    <hyperlink ref="B219" r:id="rId193" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
-    <hyperlink ref="B222" r:id="rId194" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
-    <hyperlink ref="B223" r:id="rId195" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
-    <hyperlink ref="B224" r:id="rId196" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
-    <hyperlink ref="B225" r:id="rId197" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
-    <hyperlink ref="B226" r:id="rId198" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
-    <hyperlink ref="B227" r:id="rId199" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
-    <hyperlink ref="B228" r:id="rId200" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
-    <hyperlink ref="B229" r:id="rId201" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
-    <hyperlink ref="B230" r:id="rId202" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
-    <hyperlink ref="B231" r:id="rId203" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
-    <hyperlink ref="B232" r:id="rId204" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
-    <hyperlink ref="B233" r:id="rId205" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
-    <hyperlink ref="B234" r:id="rId206" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
-    <hyperlink ref="B235" r:id="rId207" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
-    <hyperlink ref="B236" r:id="rId208" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
-    <hyperlink ref="B237" r:id="rId209" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
-    <hyperlink ref="B238" r:id="rId210" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
-    <hyperlink ref="B239" r:id="rId211" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
-    <hyperlink ref="B240" r:id="rId212" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
-    <hyperlink ref="B241" r:id="rId213" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
-    <hyperlink ref="B242" r:id="rId214" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
-    <hyperlink ref="B243" r:id="rId215" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
-    <hyperlink ref="B246" r:id="rId216" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
-    <hyperlink ref="B247" r:id="rId217" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
-    <hyperlink ref="B248" r:id="rId218" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
-    <hyperlink ref="B249" r:id="rId219" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
-    <hyperlink ref="B250" r:id="rId220" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
-    <hyperlink ref="B251" r:id="rId221" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
-    <hyperlink ref="B252" r:id="rId222" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
-    <hyperlink ref="B253" r:id="rId223" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
-    <hyperlink ref="B254" r:id="rId224" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
-    <hyperlink ref="B255" r:id="rId225" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
-    <hyperlink ref="B256" r:id="rId226" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
-    <hyperlink ref="B257" r:id="rId227" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
-    <hyperlink ref="B258" r:id="rId228" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
-    <hyperlink ref="B259" r:id="rId229" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
-    <hyperlink ref="B260" r:id="rId230" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
-    <hyperlink ref="B261" r:id="rId231" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
-    <hyperlink ref="B262" r:id="rId232" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
-    <hyperlink ref="B263" r:id="rId233" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
-    <hyperlink ref="B264" r:id="rId234" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
-    <hyperlink ref="B265" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
-    <hyperlink ref="B266" r:id="rId236" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
-    <hyperlink ref="B267" r:id="rId237" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
-    <hyperlink ref="B268" r:id="rId238" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
-    <hyperlink ref="B269" r:id="rId239" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
-    <hyperlink ref="B270" r:id="rId240" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
-    <hyperlink ref="B271" r:id="rId241" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
-    <hyperlink ref="B272" r:id="rId242" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
-    <hyperlink ref="B273" r:id="rId243" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
-    <hyperlink ref="B274" r:id="rId244" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
-    <hyperlink ref="B275" r:id="rId245" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
-    <hyperlink ref="B276" r:id="rId246" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
-    <hyperlink ref="B277" r:id="rId247" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
-    <hyperlink ref="B278" r:id="rId248" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
-    <hyperlink ref="B279" r:id="rId249" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
-    <hyperlink ref="B280" r:id="rId250" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
-    <hyperlink ref="B283" r:id="rId251" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
-    <hyperlink ref="B284" r:id="rId252" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
-    <hyperlink ref="B285" r:id="rId253" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
-    <hyperlink ref="B286" r:id="rId254" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
-    <hyperlink ref="B287" r:id="rId255" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
-    <hyperlink ref="B288" r:id="rId256" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
-    <hyperlink ref="B289" r:id="rId257" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
-    <hyperlink ref="B290" r:id="rId258" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
-    <hyperlink ref="B291" r:id="rId259" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
-    <hyperlink ref="B292" r:id="rId260" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
-    <hyperlink ref="B293" r:id="rId261" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
-    <hyperlink ref="B294" r:id="rId262" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
-    <hyperlink ref="B295" r:id="rId263" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
-    <hyperlink ref="B296" r:id="rId264" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
-    <hyperlink ref="B297" r:id="rId265" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
-    <hyperlink ref="B298" r:id="rId266" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
-    <hyperlink ref="B299" r:id="rId267" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
-    <hyperlink ref="B300" r:id="rId268" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
-    <hyperlink ref="B301" r:id="rId269" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
-    <hyperlink ref="B304" r:id="rId270" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
-    <hyperlink ref="B305" r:id="rId271" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
-    <hyperlink ref="B306" r:id="rId272" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
-    <hyperlink ref="B307" r:id="rId273" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
-    <hyperlink ref="B308" r:id="rId274" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
-    <hyperlink ref="B309" r:id="rId275" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
-    <hyperlink ref="B310" r:id="rId276" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
-    <hyperlink ref="B311" r:id="rId277" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
-    <hyperlink ref="B312" r:id="rId278" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
-    <hyperlink ref="B313" r:id="rId279" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
-    <hyperlink ref="B314" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
-    <hyperlink ref="B315" r:id="rId281" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
-    <hyperlink ref="B316" r:id="rId282" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
-    <hyperlink ref="B317" r:id="rId283" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
-    <hyperlink ref="B318" r:id="rId284" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
-    <hyperlink ref="B319" r:id="rId285" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
-    <hyperlink ref="B320" r:id="rId286" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
-    <hyperlink ref="B321" r:id="rId287" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
-    <hyperlink ref="B322" r:id="rId288" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
-    <hyperlink ref="B323" r:id="rId289" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
-    <hyperlink ref="B324" r:id="rId290" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
-    <hyperlink ref="B325" r:id="rId291" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
-    <hyperlink ref="B326" r:id="rId292" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
-    <hyperlink ref="B327" r:id="rId293" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
-    <hyperlink ref="B328" r:id="rId294" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
-    <hyperlink ref="B329" r:id="rId295" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
-    <hyperlink ref="B330" r:id="rId296" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
-    <hyperlink ref="B331" r:id="rId297" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
-    <hyperlink ref="B332" r:id="rId298" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
-    <hyperlink ref="B333" r:id="rId299" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
-    <hyperlink ref="B334" r:id="rId300" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
-    <hyperlink ref="B335" r:id="rId301" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
-    <hyperlink ref="B336" r:id="rId302" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
-    <hyperlink ref="B337" r:id="rId303" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
-    <hyperlink ref="B338" r:id="rId304" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
-    <hyperlink ref="B339" r:id="rId305" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
-    <hyperlink ref="B340" r:id="rId306" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
-    <hyperlink ref="B341" r:id="rId307" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
-    <hyperlink ref="B344" r:id="rId308" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
-    <hyperlink ref="B345" r:id="rId309" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
-    <hyperlink ref="B346" r:id="rId310" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
-    <hyperlink ref="B347" r:id="rId311" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
-    <hyperlink ref="B348" r:id="rId312" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
-    <hyperlink ref="B349" r:id="rId313" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
-    <hyperlink ref="B350" r:id="rId314" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
-    <hyperlink ref="B351" r:id="rId315" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
-    <hyperlink ref="B352" r:id="rId316" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
-    <hyperlink ref="B353" r:id="rId317" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
-    <hyperlink ref="B354" r:id="rId318" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
-    <hyperlink ref="B355" r:id="rId319" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
-    <hyperlink ref="B356" r:id="rId320" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
-    <hyperlink ref="B357" r:id="rId321" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
-    <hyperlink ref="B358" r:id="rId322" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
-    <hyperlink ref="B359" r:id="rId323" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
-    <hyperlink ref="B360" r:id="rId324" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
-    <hyperlink ref="B361" r:id="rId325" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
-    <hyperlink ref="B365" r:id="rId326" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
-    <hyperlink ref="B366" r:id="rId327" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
-    <hyperlink ref="B367" r:id="rId328" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
-    <hyperlink ref="B368" r:id="rId329" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
-    <hyperlink ref="B369" r:id="rId330" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
-    <hyperlink ref="B370" r:id="rId331" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
-    <hyperlink ref="B371" r:id="rId332" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
-    <hyperlink ref="B372" r:id="rId333" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
-    <hyperlink ref="B373" r:id="rId334" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
-    <hyperlink ref="B374" r:id="rId335" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
-    <hyperlink ref="B375" r:id="rId336" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
-    <hyperlink ref="B376" r:id="rId337" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
-    <hyperlink ref="B377" r:id="rId338" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
-    <hyperlink ref="B378" r:id="rId339" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
-    <hyperlink ref="B379" r:id="rId340" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
-    <hyperlink ref="B380" r:id="rId341" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
-    <hyperlink ref="B381" r:id="rId342" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="B382" r:id="rId343" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="B383" r:id="rId344" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="B384" r:id="rId345" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="B385" r:id="rId346" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="B386" r:id="rId347" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="B387" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="B388" r:id="rId349" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="B389" r:id="rId350" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="B390" r:id="rId351" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="B391" r:id="rId352" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="B392" r:id="rId353" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="B393" r:id="rId354" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="B394" r:id="rId355" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="B395" r:id="rId356" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="B396" r:id="rId357" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="B397" r:id="rId358" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="B398" r:id="rId359" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="B399" r:id="rId360" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="B400" r:id="rId361" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="B401" r:id="rId362" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="B402" r:id="rId363" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="B404" r:id="rId364" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="B403" r:id="rId365" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="B405" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="B406" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="B407" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B410" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B411" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B412" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B413" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B414" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B415" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B418" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B419" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B420" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B421" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B422" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B423" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B424" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B425" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B426" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B427" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B428" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B429" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B430" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B431" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B432" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B433" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B434" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B435" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B436" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B437" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B438" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B439" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B440" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B441" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B442" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B443" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B444" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B445" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B446" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B447" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B448" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B449" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B450" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B451" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B452" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B453" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B454" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B455" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B456" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B457" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B459" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B458" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B460" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B461" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B462" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B463" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B464" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B465" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B466" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B467" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B468" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B469" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B470" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B477" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B476" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B475" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B474" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B473" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B472" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B471" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B480" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B481" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B482" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B483" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B484" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B485" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B486" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B489" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B487" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B488" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="B364" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
+    <hyperlink ref="B189" r:id="rId159" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
+    <hyperlink ref="B190" r:id="rId160" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
+    <hyperlink ref="B191" r:id="rId161" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
+    <hyperlink ref="B192" r:id="rId162" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
+    <hyperlink ref="B193" r:id="rId163" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
+    <hyperlink ref="B194" r:id="rId164" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
+    <hyperlink ref="B195" r:id="rId165" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
+    <hyperlink ref="B196" r:id="rId166" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
+    <hyperlink ref="B197" r:id="rId167" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
+    <hyperlink ref="B198" r:id="rId168" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
+    <hyperlink ref="B199" r:id="rId169" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
+    <hyperlink ref="B200" r:id="rId170" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
+    <hyperlink ref="B201" r:id="rId171" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
+    <hyperlink ref="B202" r:id="rId172" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
+    <hyperlink ref="B203" r:id="rId173" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
+    <hyperlink ref="B204" r:id="rId174" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
+    <hyperlink ref="B205" r:id="rId175" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
+    <hyperlink ref="B206" r:id="rId176" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
+    <hyperlink ref="B207" r:id="rId177" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
+    <hyperlink ref="B208" r:id="rId178" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
+    <hyperlink ref="B209" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
+    <hyperlink ref="B210" r:id="rId180" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
+    <hyperlink ref="B211" r:id="rId181" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
+    <hyperlink ref="B212" r:id="rId182" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
+    <hyperlink ref="B213" r:id="rId183" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
+    <hyperlink ref="B214" r:id="rId184" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
+    <hyperlink ref="B215" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
+    <hyperlink ref="B216" r:id="rId186" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
+    <hyperlink ref="B217" r:id="rId187" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
+    <hyperlink ref="B218" r:id="rId188" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
+    <hyperlink ref="B219" r:id="rId189" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
+    <hyperlink ref="B220" r:id="rId190" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
+    <hyperlink ref="B221" r:id="rId191" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
+    <hyperlink ref="B222" r:id="rId192" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
+    <hyperlink ref="B223" r:id="rId193" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
+    <hyperlink ref="B226" r:id="rId194" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
+    <hyperlink ref="B227" r:id="rId195" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
+    <hyperlink ref="B228" r:id="rId196" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
+    <hyperlink ref="B229" r:id="rId197" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
+    <hyperlink ref="B230" r:id="rId198" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
+    <hyperlink ref="B231" r:id="rId199" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
+    <hyperlink ref="B232" r:id="rId200" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
+    <hyperlink ref="B233" r:id="rId201" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
+    <hyperlink ref="B234" r:id="rId202" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
+    <hyperlink ref="B235" r:id="rId203" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
+    <hyperlink ref="B236" r:id="rId204" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
+    <hyperlink ref="B237" r:id="rId205" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
+    <hyperlink ref="B238" r:id="rId206" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
+    <hyperlink ref="B239" r:id="rId207" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
+    <hyperlink ref="B240" r:id="rId208" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
+    <hyperlink ref="B241" r:id="rId209" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
+    <hyperlink ref="B242" r:id="rId210" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
+    <hyperlink ref="B243" r:id="rId211" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
+    <hyperlink ref="B244" r:id="rId212" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
+    <hyperlink ref="B245" r:id="rId213" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
+    <hyperlink ref="B246" r:id="rId214" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
+    <hyperlink ref="B247" r:id="rId215" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
+    <hyperlink ref="B250" r:id="rId216" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
+    <hyperlink ref="B251" r:id="rId217" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
+    <hyperlink ref="B252" r:id="rId218" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
+    <hyperlink ref="B253" r:id="rId219" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
+    <hyperlink ref="B254" r:id="rId220" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
+    <hyperlink ref="B255" r:id="rId221" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
+    <hyperlink ref="B256" r:id="rId222" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
+    <hyperlink ref="B257" r:id="rId223" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
+    <hyperlink ref="B258" r:id="rId224" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
+    <hyperlink ref="B259" r:id="rId225" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
+    <hyperlink ref="B260" r:id="rId226" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
+    <hyperlink ref="B261" r:id="rId227" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
+    <hyperlink ref="B262" r:id="rId228" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
+    <hyperlink ref="B263" r:id="rId229" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
+    <hyperlink ref="B264" r:id="rId230" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
+    <hyperlink ref="B265" r:id="rId231" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
+    <hyperlink ref="B266" r:id="rId232" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
+    <hyperlink ref="B267" r:id="rId233" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
+    <hyperlink ref="B268" r:id="rId234" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
+    <hyperlink ref="B269" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
+    <hyperlink ref="B270" r:id="rId236" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
+    <hyperlink ref="B271" r:id="rId237" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
+    <hyperlink ref="B272" r:id="rId238" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
+    <hyperlink ref="B273" r:id="rId239" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
+    <hyperlink ref="B274" r:id="rId240" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
+    <hyperlink ref="B275" r:id="rId241" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
+    <hyperlink ref="B276" r:id="rId242" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
+    <hyperlink ref="B277" r:id="rId243" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
+    <hyperlink ref="B278" r:id="rId244" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
+    <hyperlink ref="B279" r:id="rId245" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
+    <hyperlink ref="B280" r:id="rId246" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
+    <hyperlink ref="B281" r:id="rId247" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
+    <hyperlink ref="B282" r:id="rId248" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
+    <hyperlink ref="B283" r:id="rId249" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
+    <hyperlink ref="B284" r:id="rId250" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
+    <hyperlink ref="B287" r:id="rId251" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
+    <hyperlink ref="B288" r:id="rId252" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
+    <hyperlink ref="B289" r:id="rId253" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
+    <hyperlink ref="B290" r:id="rId254" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
+    <hyperlink ref="B291" r:id="rId255" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
+    <hyperlink ref="B292" r:id="rId256" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
+    <hyperlink ref="B293" r:id="rId257" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
+    <hyperlink ref="B294" r:id="rId258" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
+    <hyperlink ref="B295" r:id="rId259" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
+    <hyperlink ref="B296" r:id="rId260" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
+    <hyperlink ref="B297" r:id="rId261" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
+    <hyperlink ref="B298" r:id="rId262" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
+    <hyperlink ref="B299" r:id="rId263" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
+    <hyperlink ref="B300" r:id="rId264" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
+    <hyperlink ref="B301" r:id="rId265" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
+    <hyperlink ref="B302" r:id="rId266" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
+    <hyperlink ref="B303" r:id="rId267" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
+    <hyperlink ref="B304" r:id="rId268" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="B305" r:id="rId269" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
+    <hyperlink ref="B308" r:id="rId270" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
+    <hyperlink ref="B309" r:id="rId271" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
+    <hyperlink ref="B310" r:id="rId272" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
+    <hyperlink ref="B311" r:id="rId273" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
+    <hyperlink ref="B312" r:id="rId274" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
+    <hyperlink ref="B313" r:id="rId275" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
+    <hyperlink ref="B314" r:id="rId276" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
+    <hyperlink ref="B315" r:id="rId277" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
+    <hyperlink ref="B316" r:id="rId278" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
+    <hyperlink ref="B317" r:id="rId279" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
+    <hyperlink ref="B318" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
+    <hyperlink ref="B319" r:id="rId281" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
+    <hyperlink ref="B320" r:id="rId282" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
+    <hyperlink ref="B321" r:id="rId283" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
+    <hyperlink ref="B322" r:id="rId284" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
+    <hyperlink ref="B323" r:id="rId285" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
+    <hyperlink ref="B324" r:id="rId286" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
+    <hyperlink ref="B325" r:id="rId287" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
+    <hyperlink ref="B326" r:id="rId288" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
+    <hyperlink ref="B327" r:id="rId289" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
+    <hyperlink ref="B328" r:id="rId290" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
+    <hyperlink ref="B329" r:id="rId291" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
+    <hyperlink ref="B330" r:id="rId292" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
+    <hyperlink ref="B331" r:id="rId293" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
+    <hyperlink ref="B332" r:id="rId294" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
+    <hyperlink ref="B333" r:id="rId295" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
+    <hyperlink ref="B334" r:id="rId296" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
+    <hyperlink ref="B335" r:id="rId297" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
+    <hyperlink ref="B336" r:id="rId298" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
+    <hyperlink ref="B337" r:id="rId299" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
+    <hyperlink ref="B338" r:id="rId300" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
+    <hyperlink ref="B339" r:id="rId301" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
+    <hyperlink ref="B340" r:id="rId302" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
+    <hyperlink ref="B341" r:id="rId303" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
+    <hyperlink ref="B342" r:id="rId304" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
+    <hyperlink ref="B343" r:id="rId305" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
+    <hyperlink ref="B344" r:id="rId306" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
+    <hyperlink ref="B345" r:id="rId307" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
+    <hyperlink ref="B348" r:id="rId308" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
+    <hyperlink ref="B349" r:id="rId309" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
+    <hyperlink ref="B350" r:id="rId310" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
+    <hyperlink ref="B351" r:id="rId311" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
+    <hyperlink ref="B352" r:id="rId312" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
+    <hyperlink ref="B353" r:id="rId313" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
+    <hyperlink ref="B354" r:id="rId314" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
+    <hyperlink ref="B355" r:id="rId315" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
+    <hyperlink ref="B356" r:id="rId316" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
+    <hyperlink ref="B357" r:id="rId317" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
+    <hyperlink ref="B358" r:id="rId318" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
+    <hyperlink ref="B359" r:id="rId319" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
+    <hyperlink ref="B360" r:id="rId320" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
+    <hyperlink ref="B361" r:id="rId321" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
+    <hyperlink ref="B362" r:id="rId322" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
+    <hyperlink ref="B363" r:id="rId323" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
+    <hyperlink ref="B364" r:id="rId324" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
+    <hyperlink ref="B365" r:id="rId325" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
+    <hyperlink ref="B369" r:id="rId326" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
+    <hyperlink ref="B370" r:id="rId327" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
+    <hyperlink ref="B371" r:id="rId328" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
+    <hyperlink ref="B372" r:id="rId329" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
+    <hyperlink ref="B373" r:id="rId330" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
+    <hyperlink ref="B374" r:id="rId331" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
+    <hyperlink ref="B375" r:id="rId332" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
+    <hyperlink ref="B376" r:id="rId333" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
+    <hyperlink ref="B377" r:id="rId334" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
+    <hyperlink ref="B378" r:id="rId335" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
+    <hyperlink ref="B379" r:id="rId336" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
+    <hyperlink ref="B380" r:id="rId337" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
+    <hyperlink ref="B381" r:id="rId338" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
+    <hyperlink ref="B382" r:id="rId339" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
+    <hyperlink ref="B383" r:id="rId340" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
+    <hyperlink ref="B384" r:id="rId341" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
+    <hyperlink ref="B385" r:id="rId342" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
+    <hyperlink ref="B386" r:id="rId343" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
+    <hyperlink ref="B387" r:id="rId344" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
+    <hyperlink ref="B388" r:id="rId345" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
+    <hyperlink ref="B389" r:id="rId346" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
+    <hyperlink ref="B390" r:id="rId347" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
+    <hyperlink ref="B391" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="B392" r:id="rId349" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="B393" r:id="rId350" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="B394" r:id="rId351" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="B395" r:id="rId352" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="B396" r:id="rId353" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="B397" r:id="rId354" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="B398" r:id="rId355" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="B399" r:id="rId356" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="B400" r:id="rId357" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="B401" r:id="rId358" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="B402" r:id="rId359" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="B403" r:id="rId360" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="B404" r:id="rId361" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="B405" r:id="rId362" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="B406" r:id="rId363" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="B408" r:id="rId364" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="B407" r:id="rId365" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="B409" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="B410" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="B411" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="B414" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B415" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B416" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B417" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B418" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B419" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B422" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B423" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B424" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B425" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B426" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B427" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B428" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B429" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B430" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B431" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B432" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B433" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B434" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B435" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B436" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B437" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B438" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B439" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B440" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B441" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B442" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B443" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B444" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B445" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B446" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B447" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B448" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B449" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B450" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B451" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B452" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B453" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B454" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B455" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B456" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B457" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B458" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B459" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B460" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B461" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B463" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B462" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B464" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B465" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B466" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B467" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B468" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B469" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B470" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B471" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B472" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B473" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B474" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B481" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B480" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B479" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B478" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B477" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B476" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B475" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B484" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B485" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B486" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B487" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B488" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B489" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B490" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B493" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B491" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B492" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B368" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved "Insertion Point of 2 Linked list" from 450 DSA sheet and Striver.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9D793F-2571-42B4-B16F-6DC22103661B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D52C02-0627-4171-A5BD-8156BC1566A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1893,7 +1893,7 @@
   <dimension ref="A1:C493"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A150" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3521,7 +3521,7 @@
         <v>145</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Marked Yes in 450 DSA Sheet for "Reverse a Linked List in groups of given size"
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D52C02-0627-4171-A5BD-8156BC1566A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104323DE-6BEB-45AD-BBF6-83CA7532BEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3411,7 +3411,7 @@
         <v>135</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Updated the Final450 DSA Sheet "Clone a linked list with next and random pointer"
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104323DE-6BEB-45AD-BBF6-83CA7532BEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164C324A-8CE1-4FAC-A01A-16A1F218D397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="476">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3554,7 +3554,7 @@
         <v>148</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="21">
@@ -3719,7 +3719,7 @@
         <v>163</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="21">
@@ -3822,7 +3822,9 @@
       </c>
     </row>
     <row r="184" spans="1:3" ht="19.5">
-      <c r="A184" s="7"/>
+      <c r="A184" s="7" t="s">
+        <v>133</v>
+      </c>
       <c r="C184" s="3"/>
     </row>
     <row r="185" spans="1:3" ht="19.5">

</xml_diff>

<commit_message>
Solved 2 question from 450 DSA sheet and Striver 1) Starting point of the loop in the linked list 2) Detect a loop in the Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164C324A-8CE1-4FAC-A01A-16A1F218D397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F79FCB-8F83-497B-9724-7CE60F5E7037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C174" sqref="C174"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3422,7 +3422,7 @@
         <v>136</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="21">
@@ -3444,7 +3444,7 @@
         <v>138</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Did More question from Striver and 450 DSA sheet
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F79FCB-8F83-497B-9724-7CE60F5E7037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDFD7C1-CCA5-4042-937B-8BAF4184BF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="477">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1453,6 +1453,9 @@
   </si>
   <si>
     <t>Find Middle of the Linked List from Striver</t>
+  </si>
+  <si>
+    <t>Rotate a Linked list from Striver</t>
   </si>
 </sst>
 </file>
@@ -1892,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C150" sqref="C150"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C185" sqref="C185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3587,7 +3590,7 @@
         <v>151</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="21">
@@ -3697,7 +3700,7 @@
         <v>161</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="21">
@@ -3825,7 +3828,12 @@
       <c r="A184" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C184" s="3"/>
+      <c r="B184" t="s">
+        <v>476</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="185" spans="1:3" ht="19.5">
       <c r="A185" s="7"/>

</xml_diff>

<commit_message>
Solved "Trapping Rainwater problem" from Striver and 450 DSA Sheet TC - O(n) SC - O(1)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E96BCD4-8B1F-49E9-930D-3031BFEB096E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8062F5F-3A12-4E07-A323-DF42CE71E9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2246,7 +2246,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>3</v>
+        <v>464</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Updated 450 Excel and did some question
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8062F5F-3A12-4E07-A323-DF42CE71E9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE29C87-6130-4FB8-9341-6991704D95CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -4595,7 +4595,7 @@
         <v>237</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="261" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Marked in 450 DSA Sheet and did Equal sum Partion top down.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE29C87-6130-4FB8-9341-6991704D95CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3934445C-C6AA-455F-921A-1058BBABC161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A417" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C426" sqref="C426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -6337,7 +6337,7 @@
         <v>394</v>
       </c>
       <c r="C426" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="427" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Did Some Dynamic Programming question 1) 01 Knapsack 2) Unbounded Knapsack 3)Coin Change Problem 4)Rod Cutting Problem
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\OneDrive\Desktop\450 DSA and 30 Day Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3934445C-C6AA-455F-921A-1058BBABC161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BA6B46-E760-493A-A7DA-6F437F9BF7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A417" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C426" sqref="C426"/>
+    <sheetView tabSelected="1" topLeftCell="A286" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C433" sqref="C433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -6403,7 +6403,7 @@
         <v>272</v>
       </c>
       <c r="C432" s="3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="433" spans="1:3" ht="21">

</xml_diff>